<commit_message>
Saldo masuk dari Abudullah Tuyar
</commit_message>
<xml_diff>
--- a/Jual Pulsa.xlsx
+++ b/Jual Pulsa.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156">
   <si>
     <t>Tgl</t>
   </si>
@@ -439,6 +439,21 @@
   </si>
   <si>
     <t>Jumadi</t>
+  </si>
+  <si>
+    <t>BL171111CBC2ELC</t>
+  </si>
+  <si>
+    <t>Bagus Prasojo</t>
+  </si>
+  <si>
+    <t>520530520059</t>
+  </si>
+  <si>
+    <t>Srini</t>
+  </si>
+  <si>
+    <t>08522904326</t>
   </si>
   <si>
     <t>Tanggal</t>
@@ -479,12 +494,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -508,84 +523,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -607,7 +546,73 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -629,22 +634,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -652,7 +660,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -667,7 +675,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -679,7 +747,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -691,43 +819,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -739,97 +831,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -841,7 +849,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -913,15 +921,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -933,45 +932,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1002,6 +962,39 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1010,149 +1003,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1541,7 +1549,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H84" sqref="H84"/>
+      <selection pane="bottomLeft" activeCell="J81" sqref="J81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3301,7 +3309,7 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="19">
-        <v>43210</v>
+        <v>43211</v>
       </c>
       <c r="B77" s="15" t="s">
         <v>136</v>
@@ -3321,25 +3329,68 @@
       <c r="G77" t="s">
         <v>14</v>
       </c>
+      <c r="H77" s="23">
+        <v>51500</v>
+      </c>
       <c r="J77" s="23">
-        <v>50000</v>
+        <v>51500</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="19">
-        <v>43210</v>
-      </c>
-      <c r="B78" s="15"/>
-      <c r="F78" s="23"/>
-      <c r="J78" s="23"/>
+        <v>43211</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C78" t="s">
+        <v>141</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="E78" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="F78" s="23">
+        <v>51500</v>
+      </c>
+      <c r="G78" t="s">
+        <v>14</v>
+      </c>
+      <c r="H78" s="23">
+        <v>51500</v>
+      </c>
+      <c r="J78" s="23">
+        <v>51500</v>
+      </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" s="19">
         <v>43210</v>
       </c>
       <c r="B79" s="15"/>
-      <c r="F79" s="23"/>
-      <c r="J79" s="23"/>
+      <c r="C79" t="s">
+        <v>143</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="E79" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="F79" s="23">
+        <v>11000</v>
+      </c>
+      <c r="G79" t="s">
+        <v>10</v>
+      </c>
+      <c r="H79">
+        <v>11000</v>
+      </c>
+      <c r="J79" s="23">
+        <v>11000</v>
+      </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="19">
@@ -3510,22 +3561,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3604,7 +3655,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="7" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -3617,7 +3668,7 @@
     </row>
     <row r="9" spans="4:5">
       <c r="D9" s="11" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E9" s="12">
         <v>1000000</v>
@@ -3625,7 +3676,7 @@
     </row>
     <row r="10" spans="4:5">
       <c r="D10" s="13" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E10" s="5">
         <f>E9-E6</f>
@@ -3638,7 +3689,7 @@
     </row>
     <row r="12" spans="4:5">
       <c r="D12" s="3" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="E12" s="5">
         <v>300000</v>
@@ -3646,7 +3697,7 @@
     </row>
     <row r="13" spans="4:5">
       <c r="D13" s="13" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="E13" s="5">
         <v>300000</v>
@@ -3654,7 +3705,7 @@
     </row>
     <row r="14" spans="4:5">
       <c r="D14" s="11" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E14" s="12">
         <f>E13+E12</f>
@@ -3667,7 +3718,7 @@
     </row>
     <row r="16" spans="4:5">
       <c r="D16" s="11" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E16" s="12">
         <f>E10-E14</f>

</xml_diff>

<commit_message>
Transfer 25jt ke Abu hisyam
</commit_message>
<xml_diff>
--- a/Jual Pulsa.xlsx
+++ b/Jual Pulsa.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$I$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$I$124</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="242">
   <si>
     <t>Tgl</t>
   </si>
@@ -634,6 +634,117 @@
   </si>
   <si>
     <t xml:space="preserve">BL17112ZMBLWINV </t>
+  </si>
+  <si>
+    <t>BL171111DS6CELC</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>520530503784/14003744563</t>
+  </si>
+  <si>
+    <t>BL171111DT72ELC</t>
+  </si>
+  <si>
+    <t>BL171111DTV2ELC</t>
+  </si>
+  <si>
+    <t>520511772327/01120229651</t>
+  </si>
+  <si>
+    <t>BL171111DWT2ELC</t>
+  </si>
+  <si>
+    <t>BL171131SE82INV</t>
+  </si>
+  <si>
+    <t>082333852871</t>
+  </si>
+  <si>
+    <t>085643862422</t>
+  </si>
+  <si>
+    <t>BL171131X6IHINV</t>
+  </si>
+  <si>
+    <t>BL1711323X2HINV</t>
+  </si>
+  <si>
+    <t>081213199936</t>
+  </si>
+  <si>
+    <t>BL171131XAKMINV</t>
+  </si>
+  <si>
+    <t>BL171111EPKMELC</t>
+  </si>
+  <si>
+    <t>BL171111EPZ7ELC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BL17112ZRTEWINV </t>
+  </si>
+  <si>
+    <t>Mas Rian</t>
+  </si>
+  <si>
+    <t>087734946343</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>BL171111E4VCELC</t>
+  </si>
+  <si>
+    <t>082328564144</t>
+  </si>
+  <si>
+    <t>Abu Falih Rasyid</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BL171131SAN2INV </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BL171131SM8CINV </t>
+  </si>
+  <si>
+    <t>BL171131SUFCINV</t>
+  </si>
+  <si>
+    <t>085292997788</t>
+  </si>
+  <si>
+    <t>087836007077</t>
+  </si>
+  <si>
+    <t>BL171131WJ1WINV</t>
+  </si>
+  <si>
+    <t>BL171131Y6CHINV</t>
+  </si>
+  <si>
+    <t>BL171131ZOMCINV</t>
+  </si>
+  <si>
+    <t>085229722916</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BL171111EPJWELC </t>
+  </si>
+  <si>
+    <t>BL17112ZR1CHINV</t>
+  </si>
+  <si>
+    <t>087734946272</t>
+  </si>
+  <si>
+    <t>BL17112ZP7KHINV</t>
+  </si>
+  <si>
+    <t>089671649347</t>
   </si>
 </sst>
 </file>
@@ -643,12 +754,19 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -758,11 +876,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -770,43 +888,47 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1102,11 +1224,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N140"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:N141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F105" sqref="F105"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1114,13 +1237,13 @@
     <col min="1" max="1" width="17.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="19" style="12" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" style="12" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="17.140625" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" customWidth="1"/>
     <col min="13" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1154,7 +1277,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" hidden="1">
       <c r="A2" s="12"/>
       <c r="B2" s="16">
         <v>42825</v>
@@ -1176,7 +1299,7 @@
       </c>
       <c r="J2" s="20"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" hidden="1">
       <c r="A3" s="12"/>
       <c r="C3" t="s">
         <v>9</v>
@@ -1192,7 +1315,7 @@
       </c>
       <c r="J3" s="20"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" hidden="1">
       <c r="A4" s="12"/>
       <c r="C4" t="s">
         <v>11</v>
@@ -1208,7 +1331,7 @@
       </c>
       <c r="J4" s="20"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" hidden="1">
       <c r="A5" s="12"/>
       <c r="B5" s="16">
         <v>42825</v>
@@ -1227,7 +1350,7 @@
       </c>
       <c r="J5" s="20"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" hidden="1">
       <c r="A6" s="12"/>
       <c r="C6" t="s">
         <v>13</v>
@@ -1243,7 +1366,7 @@
       </c>
       <c r="J6" s="20"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" hidden="1">
       <c r="A7" s="12"/>
       <c r="B7" s="16">
         <v>42825</v>
@@ -1271,7 +1394,7 @@
       </c>
       <c r="J7" s="20"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" hidden="1">
       <c r="A8" s="12"/>
       <c r="B8" s="16"/>
       <c r="C8" t="s">
@@ -1285,7 +1408,7 @@
       </c>
       <c r="J8" s="20"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" hidden="1">
       <c r="A9" s="12"/>
       <c r="B9" s="16">
         <v>42826</v>
@@ -1304,7 +1427,7 @@
       </c>
       <c r="J9" s="20"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" hidden="1">
       <c r="A10" s="12"/>
       <c r="B10" s="16">
         <v>42826</v>
@@ -1323,7 +1446,7 @@
       </c>
       <c r="J10" s="20"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" hidden="1">
       <c r="A11" s="12"/>
       <c r="B11" s="16">
         <v>42826</v>
@@ -1343,7 +1466,7 @@
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" hidden="1">
       <c r="A12" s="12"/>
       <c r="B12" s="16">
         <v>42826</v>
@@ -1362,7 +1485,7 @@
       </c>
       <c r="J12" s="20"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" hidden="1">
       <c r="A13" s="12"/>
       <c r="B13" s="16">
         <v>42831</v>
@@ -1387,7 +1510,7 @@
       </c>
       <c r="J13" s="20"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" hidden="1">
       <c r="A14" s="12"/>
       <c r="B14" s="16">
         <v>42831</v>
@@ -1406,7 +1529,7 @@
       </c>
       <c r="J14" s="20"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" hidden="1">
       <c r="A15" s="12"/>
       <c r="B15" s="16">
         <v>42831</v>
@@ -1431,7 +1554,7 @@
       </c>
       <c r="J15" s="20"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" hidden="1">
       <c r="A16" s="12"/>
       <c r="B16" s="16">
         <v>42831</v>
@@ -1450,7 +1573,7 @@
       </c>
       <c r="J16" s="20"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" hidden="1">
       <c r="A17" s="12"/>
       <c r="B17" s="16">
         <v>42832</v>
@@ -1469,7 +1592,7 @@
       </c>
       <c r="J17" s="20"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" hidden="1">
       <c r="A18" s="12"/>
       <c r="B18" s="16">
         <v>42832</v>
@@ -1489,7 +1612,7 @@
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" hidden="1">
       <c r="A19" s="12"/>
       <c r="B19" s="16">
         <v>42832</v>
@@ -1517,7 +1640,7 @@
       </c>
       <c r="J19" s="20"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" hidden="1">
       <c r="A20" s="12"/>
       <c r="B20" s="16">
         <v>42832</v>
@@ -1539,7 +1662,7 @@
       </c>
       <c r="J20" s="20"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" hidden="1">
       <c r="A21" s="12"/>
       <c r="B21" s="16">
         <v>42833</v>
@@ -1567,7 +1690,7 @@
       </c>
       <c r="J21" s="20"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" hidden="1">
       <c r="A22" s="12"/>
       <c r="B22" s="16">
         <v>42833</v>
@@ -1595,7 +1718,7 @@
       </c>
       <c r="J22" s="20"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" hidden="1">
       <c r="A23" s="12"/>
       <c r="B23" s="16">
         <v>42833</v>
@@ -1623,7 +1746,7 @@
       </c>
       <c r="J23" s="20"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" hidden="1">
       <c r="A24" s="12"/>
       <c r="B24" s="16">
         <v>42833</v>
@@ -1642,7 +1765,7 @@
       </c>
       <c r="J24" s="20"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" hidden="1">
       <c r="A25" s="12"/>
       <c r="B25" s="16">
         <v>42833</v>
@@ -1667,7 +1790,7 @@
       </c>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" hidden="1">
       <c r="A26" s="12"/>
       <c r="B26" s="16">
         <v>42833</v>
@@ -1686,7 +1809,7 @@
       </c>
       <c r="J26" s="20"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" hidden="1">
       <c r="A27" s="12"/>
       <c r="B27" s="16">
         <v>42834</v>
@@ -1705,7 +1828,7 @@
       </c>
       <c r="J27" s="20"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" hidden="1">
       <c r="A28" s="12"/>
       <c r="B28" s="16">
         <v>42834</v>
@@ -1734,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" hidden="1">
       <c r="A29" s="12"/>
       <c r="B29" s="16">
         <v>42834</v>
@@ -1765,7 +1888,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" hidden="1">
       <c r="A30" s="12"/>
       <c r="B30" s="16">
         <v>42834</v>
@@ -1788,7 +1911,7 @@
       <c r="J30" s="20"/>
       <c r="L30" s="19"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" hidden="1">
       <c r="A31" s="12"/>
       <c r="B31" s="16">
         <v>42834</v>
@@ -1816,7 +1939,7 @@
       </c>
       <c r="J31" s="20"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" hidden="1">
       <c r="A32" s="12"/>
       <c r="B32" s="16">
         <v>42835</v>
@@ -1844,7 +1967,7 @@
       </c>
       <c r="J32" s="20"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" hidden="1">
       <c r="A33" s="12"/>
       <c r="B33" s="16">
         <v>42835</v>
@@ -1872,7 +1995,7 @@
       </c>
       <c r="J33" s="20"/>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" hidden="1">
       <c r="A34" s="12"/>
       <c r="B34" s="16">
         <v>42836</v>
@@ -1891,7 +2014,7 @@
       </c>
       <c r="J34" s="20"/>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" hidden="1">
       <c r="A35" s="12"/>
       <c r="B35" s="16">
         <v>42836</v>
@@ -1919,7 +2042,7 @@
       </c>
       <c r="J35" s="20"/>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" hidden="1">
       <c r="A36" s="12"/>
       <c r="B36" s="16">
         <v>42837</v>
@@ -1941,7 +2064,7 @@
       </c>
       <c r="J36" s="20"/>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" hidden="1">
       <c r="A37" s="12"/>
       <c r="B37" s="16">
         <v>42837</v>
@@ -1963,7 +2086,7 @@
       </c>
       <c r="J37" s="20"/>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" hidden="1">
       <c r="A38" s="12"/>
       <c r="B38" s="16">
         <v>42838</v>
@@ -1988,7 +2111,7 @@
       </c>
       <c r="J38" s="20"/>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" hidden="1">
       <c r="A39" s="12"/>
       <c r="B39" s="16">
         <v>42838</v>
@@ -2011,10 +2134,12 @@
       <c r="H39" s="17">
         <v>51500</v>
       </c>
-      <c r="I39" s="20"/>
+      <c r="I39" s="20">
+        <v>50000</v>
+      </c>
       <c r="J39" s="20"/>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" hidden="1">
       <c r="A40" s="12"/>
       <c r="B40" s="16">
         <v>42838</v>
@@ -2037,7 +2162,7 @@
       <c r="I40" s="20"/>
       <c r="J40" s="20"/>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" hidden="1">
       <c r="A41" s="12"/>
       <c r="B41" s="16">
         <v>42839</v>
@@ -2062,7 +2187,7 @@
       </c>
       <c r="J41" s="20"/>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" hidden="1">
       <c r="A42" s="12"/>
       <c r="B42" s="16">
         <v>42839</v>
@@ -2087,7 +2212,7 @@
       </c>
       <c r="J42" s="20"/>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" hidden="1">
       <c r="A43" s="12"/>
       <c r="B43" s="16">
         <v>42839</v>
@@ -2116,7 +2241,7 @@
       <c r="J43" s="20"/>
       <c r="L43" s="19"/>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" hidden="1">
       <c r="A44" s="12"/>
       <c r="B44" s="16">
         <v>42840</v>
@@ -2139,11 +2264,13 @@
       <c r="H44" s="19">
         <v>51500</v>
       </c>
-      <c r="I44" s="20"/>
+      <c r="I44" s="20">
+        <v>50000</v>
+      </c>
       <c r="J44" s="20"/>
       <c r="L44" s="19"/>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" hidden="1">
       <c r="A45" s="12"/>
       <c r="B45" s="16">
         <v>42840</v>
@@ -2171,7 +2298,7 @@
       </c>
       <c r="J45" s="20"/>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" hidden="1">
       <c r="A46" s="12"/>
       <c r="B46" s="16">
         <v>42840</v>
@@ -2191,10 +2318,12 @@
       <c r="H46" s="19">
         <v>5000</v>
       </c>
-      <c r="I46" s="20"/>
+      <c r="I46" s="20">
+        <v>6000</v>
+      </c>
       <c r="J46" s="20"/>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" hidden="1">
       <c r="A47" s="12"/>
       <c r="B47" s="16">
         <v>42840</v>
@@ -2219,7 +2348,7 @@
       </c>
       <c r="J47" s="20"/>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" hidden="1">
       <c r="A48" s="12"/>
       <c r="B48" s="16">
         <v>42840</v>
@@ -2242,7 +2371,7 @@
       <c r="I48" s="20"/>
       <c r="J48" s="20"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" hidden="1">
       <c r="A49" s="12"/>
       <c r="B49" s="16">
         <v>42841</v>
@@ -2270,7 +2399,7 @@
       </c>
       <c r="J49" s="20"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" hidden="1">
       <c r="A50" s="12"/>
       <c r="B50" s="16">
         <v>42841</v>
@@ -2298,7 +2427,7 @@
       </c>
       <c r="J50" s="20"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" hidden="1">
       <c r="A51" s="12"/>
       <c r="B51" s="16">
         <v>42841</v>
@@ -2326,7 +2455,7 @@
       </c>
       <c r="J51" s="20"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" hidden="1">
       <c r="A52" s="12"/>
       <c r="B52" s="16">
         <v>42841</v>
@@ -2346,10 +2475,12 @@
       <c r="H52" s="19">
         <v>36000</v>
       </c>
-      <c r="I52" s="20"/>
+      <c r="I52" s="20">
+        <v>36000</v>
+      </c>
       <c r="J52" s="20"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" hidden="1">
       <c r="A53" s="12"/>
       <c r="B53" s="16">
         <v>42841</v>
@@ -2374,7 +2505,7 @@
       </c>
       <c r="J53" s="20"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" hidden="1">
       <c r="A54" s="12"/>
       <c r="B54" s="16">
         <v>42841</v>
@@ -2402,7 +2533,7 @@
       </c>
       <c r="J54" s="20"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" hidden="1">
       <c r="A55" s="12"/>
       <c r="B55" s="16">
         <v>42841</v>
@@ -2430,7 +2561,7 @@
       </c>
       <c r="J55" s="20"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" hidden="1">
       <c r="A56" s="12"/>
       <c r="B56" s="16">
         <v>42842</v>
@@ -2455,7 +2586,7 @@
       </c>
       <c r="J56" s="20"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" hidden="1">
       <c r="A57" s="12"/>
       <c r="B57" s="16">
         <v>42842</v>
@@ -2483,7 +2614,7 @@
       </c>
       <c r="J57" s="20"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" hidden="1">
       <c r="A58" s="12"/>
       <c r="B58" s="16">
         <v>42842</v>
@@ -2511,7 +2642,7 @@
       </c>
       <c r="J58" s="20"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" hidden="1">
       <c r="A59" s="12"/>
       <c r="B59" s="16">
         <v>42842</v>
@@ -2536,7 +2667,7 @@
       </c>
       <c r="J59" s="20"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" hidden="1">
       <c r="A60" s="12"/>
       <c r="B60" s="16">
         <v>42843</v>
@@ -2564,7 +2695,7 @@
       </c>
       <c r="J60" s="20"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" hidden="1">
       <c r="A61" s="12"/>
       <c r="B61" s="16">
         <v>42843</v>
@@ -2587,10 +2718,12 @@
       <c r="H61" s="19">
         <v>51500</v>
       </c>
-      <c r="I61" s="20"/>
+      <c r="I61" s="20">
+        <v>50000</v>
+      </c>
       <c r="J61" s="20"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" hidden="1">
       <c r="A62" s="12"/>
       <c r="B62" s="16">
         <v>42843</v>
@@ -2618,7 +2751,7 @@
       </c>
       <c r="J62" s="20"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" hidden="1">
       <c r="A63" s="12"/>
       <c r="B63" s="16">
         <v>42844</v>
@@ -2666,7 +2799,7 @@
       <c r="I64" s="20"/>
       <c r="J64" s="20"/>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" hidden="1">
       <c r="A65" s="12"/>
       <c r="B65" s="16">
         <v>42844</v>
@@ -2694,7 +2827,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" hidden="1">
       <c r="A66" s="12"/>
       <c r="B66" s="16">
         <v>42844</v>
@@ -2722,7 +2855,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" hidden="1">
       <c r="A67" s="12"/>
       <c r="B67" s="16">
         <v>42844</v>
@@ -2750,7 +2883,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" hidden="1">
       <c r="A68" s="12"/>
       <c r="B68" s="16">
         <v>42844</v>
@@ -2778,7 +2911,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" hidden="1">
       <c r="A69" s="12"/>
       <c r="B69" s="16">
         <v>42844</v>
@@ -2806,7 +2939,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" hidden="1">
       <c r="A70" s="12"/>
       <c r="B70" s="16">
         <v>42844</v>
@@ -2829,7 +2962,7 @@
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" hidden="1">
       <c r="A71" s="12" t="s">
         <v>120</v>
       </c>
@@ -2856,7 +2989,7 @@
       </c>
       <c r="J71" s="20"/>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" hidden="1">
       <c r="A72" s="12" t="s">
         <v>123</v>
       </c>
@@ -2886,7 +3019,7 @@
       </c>
       <c r="J72" s="20"/>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:12" hidden="1">
       <c r="A73" s="12"/>
       <c r="B73" s="16">
         <v>42845</v>
@@ -2912,7 +3045,7 @@
       <c r="I73" s="20"/>
       <c r="J73" s="20"/>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" hidden="1">
       <c r="A74" s="12"/>
       <c r="B74" s="16">
         <v>42845</v>
@@ -2940,7 +3073,7 @@
       </c>
       <c r="J74" s="20"/>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" hidden="1">
       <c r="A75" s="12" t="s">
         <v>131</v>
       </c>
@@ -2962,10 +3095,12 @@
       <c r="H75" s="19">
         <v>24500</v>
       </c>
-      <c r="I75" s="20"/>
+      <c r="I75" s="20">
+        <v>25500</v>
+      </c>
       <c r="J75" s="20"/>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:12" hidden="1">
       <c r="A76" s="12" t="s">
         <v>133</v>
       </c>
@@ -2987,10 +3122,12 @@
       <c r="H76" s="19">
         <v>10000</v>
       </c>
-      <c r="I76" s="20"/>
+      <c r="I76" s="20">
+        <v>11000</v>
+      </c>
       <c r="J76" s="20"/>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:12" hidden="1">
       <c r="A77" s="12" t="s">
         <v>135</v>
       </c>
@@ -3020,7 +3157,7 @@
       </c>
       <c r="J77" s="20"/>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:12" hidden="1">
       <c r="A78" s="12" t="s">
         <v>139</v>
       </c>
@@ -3050,7 +3187,7 @@
       </c>
       <c r="J78" s="20"/>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:12" hidden="1">
       <c r="A79" s="12" t="s">
         <v>174</v>
       </c>
@@ -3080,7 +3217,7 @@
       </c>
       <c r="J79" s="20"/>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:12" hidden="1">
       <c r="A80" s="12" t="s">
         <v>154</v>
       </c>
@@ -3105,10 +3242,12 @@
       <c r="H80" s="20">
         <v>201500</v>
       </c>
-      <c r="I80" s="20"/>
+      <c r="I80" s="20">
+        <v>200000</v>
+      </c>
       <c r="J80" s="20"/>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:14" hidden="1">
       <c r="A81" s="12" t="s">
         <v>155</v>
       </c>
@@ -3136,7 +3275,7 @@
       <c r="I81" s="20"/>
       <c r="J81" s="20"/>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:14" hidden="1">
       <c r="A82" s="12" t="s">
         <v>159</v>
       </c>
@@ -3161,10 +3300,12 @@
       <c r="H82" s="20">
         <v>51500</v>
       </c>
-      <c r="I82" s="20"/>
+      <c r="I82" s="20">
+        <v>50000</v>
+      </c>
       <c r="J82" s="20"/>
     </row>
-    <row r="83" spans="1:14">
+    <row r="83" spans="1:14" hidden="1">
       <c r="A83" s="12" t="s">
         <v>162</v>
       </c>
@@ -3194,7 +3335,7 @@
       </c>
       <c r="J83" s="20"/>
     </row>
-    <row r="84" spans="1:14">
+    <row r="84" spans="1:14" hidden="1">
       <c r="A84" s="12" t="s">
         <v>167</v>
       </c>
@@ -3219,10 +3360,12 @@
       <c r="H84" s="20">
         <v>51500</v>
       </c>
-      <c r="I84" s="20"/>
+      <c r="I84" s="20">
+        <v>50000</v>
+      </c>
       <c r="J84" s="20"/>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:14" hidden="1">
       <c r="A85" s="12" t="s">
         <v>168</v>
       </c>
@@ -3244,10 +3387,12 @@
       <c r="H85" s="20">
         <v>5000</v>
       </c>
-      <c r="I85" s="20"/>
+      <c r="I85" s="20">
+        <v>6000</v>
+      </c>
       <c r="J85" s="20"/>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:14" hidden="1">
       <c r="A86" s="12" t="s">
         <v>171</v>
       </c>
@@ -3274,7 +3419,7 @@
       </c>
       <c r="J86" s="20"/>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:14" hidden="1">
       <c r="A87" s="12" t="s">
         <v>172</v>
       </c>
@@ -3296,18 +3441,20 @@
       <c r="H87" s="20">
         <v>49400</v>
       </c>
-      <c r="I87" s="20"/>
+      <c r="I87" s="20">
+        <v>50000</v>
+      </c>
       <c r="J87" s="20"/>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:14" hidden="1">
       <c r="A88" s="12" t="s">
         <v>176</v>
       </c>
       <c r="B88" s="16">
         <v>42847</v>
       </c>
-      <c r="C88" t="s">
-        <v>177</v>
+      <c r="C88" s="30" t="s">
+        <v>82</v>
       </c>
       <c r="D88" s="12" t="s">
         <v>175</v>
@@ -3321,10 +3468,12 @@
       <c r="H88" s="20">
         <v>5000</v>
       </c>
-      <c r="I88" s="20"/>
+      <c r="I88" s="20">
+        <v>6000</v>
+      </c>
       <c r="J88" s="20"/>
     </row>
-    <row r="89" spans="1:14">
+    <row r="89" spans="1:14" hidden="1">
       <c r="A89" s="12" t="s">
         <v>179</v>
       </c>
@@ -3349,7 +3498,7 @@
       <c r="I89" s="20"/>
       <c r="J89" s="20"/>
     </row>
-    <row r="90" spans="1:14">
+    <row r="90" spans="1:14" hidden="1">
       <c r="A90" s="12" t="s">
         <v>180</v>
       </c>
@@ -3379,7 +3528,7 @@
       </c>
       <c r="J90" s="20"/>
     </row>
-    <row r="91" spans="1:14">
+    <row r="91" spans="1:14" hidden="1">
       <c r="A91" s="12" t="s">
         <v>181</v>
       </c>
@@ -3409,7 +3558,7 @@
       </c>
       <c r="J91" s="20"/>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:14" hidden="1">
       <c r="A92" s="22" t="s">
         <v>185</v>
       </c>
@@ -3470,7 +3619,7 @@
       <c r="I93" s="20"/>
       <c r="J93" s="20"/>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:14" hidden="1">
       <c r="A94" s="22" t="s">
         <v>190</v>
       </c>
@@ -3492,10 +3641,12 @@
       <c r="H94" s="20">
         <v>24900</v>
       </c>
-      <c r="I94" s="20"/>
+      <c r="I94" s="20">
+        <v>26000</v>
+      </c>
       <c r="J94" s="20"/>
     </row>
-    <row r="95" spans="1:14">
+    <row r="95" spans="1:14" hidden="1">
       <c r="A95" t="s">
         <v>199</v>
       </c>
@@ -3547,7 +3698,7 @@
       <c r="I96" s="20"/>
       <c r="J96" s="20"/>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" hidden="1">
       <c r="A97" s="22" t="s">
         <v>196</v>
       </c>
@@ -3572,7 +3723,7 @@
       <c r="I97" s="20"/>
       <c r="J97" s="20"/>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" hidden="1">
       <c r="A98" s="22" t="s">
         <v>198</v>
       </c>
@@ -3597,14 +3748,14 @@
       <c r="I98" s="20"/>
       <c r="J98" s="20"/>
     </row>
-    <row r="99" spans="1:10">
-      <c r="A99" s="28" t="s">
+    <row r="99" spans="1:10" hidden="1">
+      <c r="A99" s="25" t="s">
         <v>201</v>
       </c>
       <c r="B99" s="16">
         <v>42851</v>
       </c>
-      <c r="C99" s="29" t="s">
+      <c r="C99" s="26" t="s">
         <v>47</v>
       </c>
       <c r="D99" s="12" t="s">
@@ -3613,7 +3764,7 @@
       <c r="F99" s="20">
         <v>25500</v>
       </c>
-      <c r="G99" s="29" t="s">
+      <c r="G99" s="26" t="s">
         <v>10</v>
       </c>
       <c r="H99" s="20">
@@ -3622,14 +3773,14 @@
       <c r="I99" s="20"/>
       <c r="J99" s="20"/>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" hidden="1">
       <c r="A100" t="s">
         <v>202</v>
       </c>
       <c r="B100" s="16">
         <v>42851</v>
       </c>
-      <c r="C100" s="29" t="s">
+      <c r="C100" s="26" t="s">
         <v>82</v>
       </c>
       <c r="D100" s="12" t="s">
@@ -3638,7 +3789,7 @@
       <c r="F100" s="20">
         <v>6000</v>
       </c>
-      <c r="G100" s="29" t="s">
+      <c r="G100" s="26" t="s">
         <v>10</v>
       </c>
       <c r="H100" s="20">
@@ -3647,14 +3798,14 @@
       <c r="I100" s="20"/>
       <c r="J100" s="20"/>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" hidden="1">
       <c r="A101" t="s">
         <v>203</v>
       </c>
       <c r="B101" s="16">
         <v>42851</v>
       </c>
-      <c r="C101" s="29" t="s">
+      <c r="C101" s="26" t="s">
         <v>82</v>
       </c>
       <c r="D101" s="12" t="s">
@@ -3663,7 +3814,7 @@
       <c r="F101" s="20">
         <v>6000</v>
       </c>
-      <c r="G101" s="29" t="s">
+      <c r="G101" s="26" t="s">
         <v>10</v>
       </c>
       <c r="H101" s="20">
@@ -3672,14 +3823,14 @@
       <c r="I101" s="20"/>
       <c r="J101" s="20"/>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" hidden="1">
       <c r="A102" t="s">
         <v>204</v>
       </c>
       <c r="B102" s="16">
         <v>42851</v>
       </c>
-      <c r="C102" s="29" t="s">
+      <c r="C102" s="26" t="s">
         <v>9</v>
       </c>
       <c r="D102" s="12" t="s">
@@ -3688,7 +3839,7 @@
       <c r="F102" s="20">
         <v>21000</v>
       </c>
-      <c r="G102" s="29" t="s">
+      <c r="G102" s="26" t="s">
         <v>10</v>
       </c>
       <c r="H102" s="20">
@@ -3697,117 +3848,586 @@
       <c r="I102" s="20"/>
       <c r="J102" s="20"/>
     </row>
-    <row r="103" spans="1:10">
-      <c r="A103" s="12"/>
+    <row r="103" spans="1:10" hidden="1">
+      <c r="A103" s="31" t="s">
+        <v>205</v>
+      </c>
       <c r="B103" s="16">
-        <v>42851</v>
+        <v>42852</v>
+      </c>
+      <c r="C103" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="D103" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="F103" s="20">
+        <v>50000</v>
+      </c>
+      <c r="G103" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H103" s="20">
+        <v>51500</v>
       </c>
       <c r="I103" s="20"/>
       <c r="J103" s="20"/>
     </row>
-    <row r="104" spans="1:10">
-      <c r="A104" s="12"/>
+    <row r="104" spans="1:10" hidden="1">
+      <c r="A104" s="31" t="s">
+        <v>208</v>
+      </c>
       <c r="B104" s="16">
-        <v>42851</v>
-      </c>
-      <c r="I104" s="20"/>
+        <v>42852</v>
+      </c>
+      <c r="C104" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D104" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E104" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F104" s="20">
+        <v>200000</v>
+      </c>
+      <c r="G104" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H104" s="20">
+        <v>201500</v>
+      </c>
+      <c r="I104" s="20">
+        <v>200000</v>
+      </c>
       <c r="J104" s="20"/>
     </row>
-    <row r="105" spans="1:10">
-      <c r="A105" s="12"/>
-      <c r="I105" s="20"/>
+    <row r="105" spans="1:10" hidden="1">
+      <c r="A105" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="B105" s="16">
+        <v>42852</v>
+      </c>
+      <c r="C105" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="D105" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="E105" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="F105" s="20">
+        <v>100000</v>
+      </c>
+      <c r="G105" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H105" s="20">
+        <v>101500</v>
+      </c>
+      <c r="I105" s="20">
+        <v>100000</v>
+      </c>
       <c r="J105" s="20"/>
     </row>
-    <row r="106" spans="1:10">
-      <c r="A106" s="12"/>
+    <row r="106" spans="1:10" hidden="1">
+      <c r="A106" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="B106" s="16">
+        <v>42852</v>
+      </c>
+      <c r="C106" t="s">
+        <v>19</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E106" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F106" s="20">
+        <v>100000</v>
+      </c>
+      <c r="G106" t="s">
+        <v>14</v>
+      </c>
+      <c r="H106" s="20">
+        <v>101500</v>
+      </c>
       <c r="I106" s="20"/>
       <c r="J106" s="20"/>
     </row>
-    <row r="107" spans="1:10">
-      <c r="I107" s="20"/>
+    <row r="107" spans="1:10" hidden="1">
+      <c r="A107" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="B107" s="16">
+        <v>42855</v>
+      </c>
+      <c r="C107" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="D107" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="F107" s="20">
+        <v>12000</v>
+      </c>
+      <c r="G107" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H107" s="20">
+        <v>11300</v>
+      </c>
       <c r="J107" s="20"/>
     </row>
-    <row r="108" spans="1:10">
-      <c r="I108" s="20"/>
+    <row r="108" spans="1:10" hidden="1">
+      <c r="A108" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="B108" s="16">
+        <v>42855</v>
+      </c>
+      <c r="C108" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D108" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="F108" s="20">
+        <v>50500</v>
+      </c>
+      <c r="G108" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H108" s="20">
+        <v>49500</v>
+      </c>
       <c r="J108" s="20"/>
     </row>
-    <row r="109" spans="1:10">
-      <c r="I109" s="20"/>
+    <row r="109" spans="1:10" hidden="1">
+      <c r="A109" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="B109" s="16">
+        <v>42855</v>
+      </c>
+      <c r="C109" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D109" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="F109" s="20">
+        <v>12000</v>
+      </c>
+      <c r="G109" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H109" s="20">
+        <v>11300</v>
+      </c>
       <c r="J109" s="20"/>
     </row>
-    <row r="110" spans="1:10">
-      <c r="I110" s="20"/>
-      <c r="J110" s="20"/>
-    </row>
-    <row r="111" spans="1:10">
+    <row r="110" spans="1:10" hidden="1">
+      <c r="A110" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="B110" s="16">
+        <v>42855</v>
+      </c>
+      <c r="C110" t="s">
+        <v>28</v>
+      </c>
+      <c r="D110" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E110" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F110" s="20">
+        <v>200000</v>
+      </c>
+      <c r="G110" t="s">
+        <v>14</v>
+      </c>
+      <c r="H110">
+        <v>201500</v>
+      </c>
+      <c r="I110" s="20">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" hidden="1">
+      <c r="A111" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="B111" s="16">
+        <v>42855</v>
+      </c>
+      <c r="C111" t="s">
+        <v>59</v>
+      </c>
+      <c r="D111" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E111" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F111" s="20">
+        <v>200000</v>
+      </c>
+      <c r="G111" t="s">
+        <v>14</v>
+      </c>
+      <c r="H111">
+        <v>201500</v>
+      </c>
       <c r="I111" s="20"/>
-      <c r="J111" s="20"/>
-    </row>
-    <row r="112" spans="1:10">
+    </row>
+    <row r="112" spans="1:10" hidden="1">
+      <c r="A112" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="B112" s="16">
+        <v>42852</v>
+      </c>
+      <c r="C112" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="D112" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="F112" s="20">
+        <v>54000</v>
+      </c>
+      <c r="G112" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="H112" s="20">
+        <v>53100</v>
+      </c>
       <c r="I112" s="20"/>
-      <c r="J112" s="20"/>
-    </row>
-    <row r="113" spans="9:10">
+    </row>
+    <row r="113" spans="1:10" hidden="1">
+      <c r="A113" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="B113" s="16">
+        <v>42853</v>
+      </c>
+      <c r="C113" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="D113" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E113" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="F113" s="20">
+        <v>200000</v>
+      </c>
+      <c r="G113" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H113" s="20">
+        <v>201500</v>
+      </c>
       <c r="I113" s="20"/>
-      <c r="J113" s="20"/>
-    </row>
-    <row r="114" spans="9:10">
+    </row>
+    <row r="114" spans="1:10" hidden="1">
+      <c r="A114" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="B114" s="16">
+        <v>42855</v>
+      </c>
+      <c r="C114" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D114" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="E114" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="F114" s="20">
+        <v>25500</v>
+      </c>
+      <c r="G114" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H114" s="20">
+        <v>24800</v>
+      </c>
       <c r="I114" s="20"/>
-      <c r="J114" s="20"/>
-    </row>
-    <row r="115" spans="9:10">
-      <c r="I115" s="20"/>
-      <c r="J115" s="20"/>
-    </row>
-    <row r="116" spans="9:10">
+    </row>
+    <row r="115" spans="1:10" hidden="1">
+      <c r="A115" s="33" t="s">
+        <v>229</v>
+      </c>
+      <c r="B115" s="16">
+        <v>42855</v>
+      </c>
+      <c r="C115" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D115" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F115" s="20">
+        <v>50500</v>
+      </c>
+      <c r="G115" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H115" s="20">
+        <v>49500</v>
+      </c>
+      <c r="I115" s="20">
+        <v>50500</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" hidden="1">
+      <c r="A116" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="B116" s="16">
+        <v>42855</v>
+      </c>
+      <c r="C116" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="D116" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="F116" s="20">
+        <v>12000</v>
+      </c>
+      <c r="G116" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H116" s="20">
+        <v>11300</v>
+      </c>
       <c r="I116" s="20"/>
-      <c r="J116" s="20"/>
-    </row>
-    <row r="117" spans="9:10">
+    </row>
+    <row r="117" spans="1:10" hidden="1">
+      <c r="A117" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="B117" s="16">
+        <v>42855</v>
+      </c>
+      <c r="C117" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="D117" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="F117" s="20">
+        <v>12000</v>
+      </c>
+      <c r="G117" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H117" s="20">
+        <v>11300</v>
+      </c>
       <c r="I117" s="20"/>
-      <c r="J117" s="20"/>
-    </row>
-    <row r="118" spans="9:10">
+    </row>
+    <row r="118" spans="1:10" hidden="1">
+      <c r="A118" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="B118" s="16">
+        <v>42855</v>
+      </c>
+      <c r="C118" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D118" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="F118" s="20">
+        <v>11000</v>
+      </c>
+      <c r="G118" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H118" s="20">
+        <v>10300</v>
+      </c>
       <c r="I118" s="20"/>
-      <c r="J118" s="20"/>
-    </row>
-    <row r="119" spans="9:10">
+    </row>
+    <row r="119" spans="1:10" hidden="1">
+      <c r="A119" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="B119" s="16">
+        <v>42855</v>
+      </c>
+      <c r="C119" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D119" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="F119" s="20">
+        <v>12000</v>
+      </c>
+      <c r="G119" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H119" s="20">
+        <v>11300</v>
+      </c>
       <c r="I119" s="20"/>
-      <c r="J119" s="20"/>
-    </row>
-    <row r="120" spans="9:10">
+    </row>
+    <row r="120" spans="1:10" hidden="1">
+      <c r="A120" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="B120" s="16">
+        <v>42855</v>
+      </c>
+      <c r="C120" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D120" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E120" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="F120" s="20">
+        <v>200000</v>
+      </c>
+      <c r="G120" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H120" s="20">
+        <v>201500</v>
+      </c>
       <c r="I120" s="20"/>
-      <c r="J120" s="20"/>
-    </row>
-    <row r="121" spans="9:10">
-      <c r="I121" s="20"/>
-      <c r="J121" s="20"/>
-    </row>
-    <row r="122" spans="9:10">
+    </row>
+    <row r="121" spans="1:10" hidden="1">
+      <c r="A121" s="12"/>
+      <c r="B121" s="16">
+        <v>42855</v>
+      </c>
+      <c r="C121" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="D121" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="E121" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="F121" s="20">
+        <v>50000</v>
+      </c>
+      <c r="G121" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H121" s="20">
+        <v>51500</v>
+      </c>
+      <c r="I121" s="20">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" hidden="1">
+      <c r="A122" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="B122" s="16">
+        <v>42856</v>
+      </c>
+      <c r="C122" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D122" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="F122" s="20">
+        <v>12000</v>
+      </c>
+      <c r="G122" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="H122" s="20">
+        <v>11300</v>
+      </c>
       <c r="I122" s="20"/>
-      <c r="J122" s="20"/>
-    </row>
-    <row r="123" spans="9:10">
+    </row>
+    <row r="123" spans="1:10" hidden="1">
+      <c r="A123" s="33" t="s">
+        <v>238</v>
+      </c>
+      <c r="B123" s="16">
+        <v>42852</v>
+      </c>
+      <c r="C123" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="D123" s="31" t="s">
+        <v>239</v>
+      </c>
+      <c r="F123" s="20">
+        <v>54000</v>
+      </c>
+      <c r="G123" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="H123" s="20">
+        <v>53100</v>
+      </c>
       <c r="I123" s="20"/>
-      <c r="J123" s="20"/>
-    </row>
-    <row r="124" spans="9:10">
+    </row>
+    <row r="124" spans="1:10" hidden="1">
+      <c r="A124" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="B124" s="16">
+        <v>42852</v>
+      </c>
+      <c r="C124" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="D124" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="F124" s="20">
+        <v>11000</v>
+      </c>
+      <c r="G124" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H124" s="20">
+        <v>10000</v>
+      </c>
       <c r="I124" s="20"/>
-      <c r="J124" s="20"/>
-    </row>
-    <row r="125" spans="9:10">
+    </row>
+    <row r="125" spans="1:10">
       <c r="I125" s="20"/>
       <c r="J125" s="20"/>
     </row>
-    <row r="126" spans="9:10">
+    <row r="126" spans="1:10">
       <c r="I126" s="20"/>
       <c r="J126" s="20"/>
     </row>
-    <row r="127" spans="9:10">
+    <row r="127" spans="1:10">
       <c r="I127" s="20"/>
       <c r="J127" s="20"/>
     </row>
-    <row r="128" spans="9:10">
+    <row r="128" spans="1:10">
       <c r="I128" s="20"/>
       <c r="J128" s="20"/>
     </row>
@@ -3859,14 +4479,25 @@
       <c r="I140" s="20"/>
       <c r="J140" s="20"/>
     </row>
+    <row r="141" spans="9:10">
+      <c r="I141" s="20"/>
+      <c r="J141" s="20"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:I98">
+  <autoFilter ref="B1:I124">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Rohmadi"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="4"/>
     <filterColumn colId="5"/>
-    <filterColumn colId="7"/>
+    <filterColumn colId="7">
+      <filters blank="1"/>
+    </filterColumn>
   </autoFilter>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3995,12 +4626,12 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="7">
         <f>SUM(E2:E5)</f>
         <v>137000</v>

</xml_diff>

<commit_message>
BL 31 Mei blm sls
</commit_message>
<xml_diff>
--- a/Jual Pulsa.xlsx
+++ b/Jual Pulsa.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$I$265</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$I$308</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530">
   <si>
     <t>No Transaksi</t>
   </si>
@@ -1423,6 +1423,126 @@
   </si>
   <si>
     <t>BL17113CCQIXINV</t>
+  </si>
+  <si>
+    <t>BL171111TBBIELC</t>
+  </si>
+  <si>
+    <t>BL17113CGXX3INV</t>
+  </si>
+  <si>
+    <t>BL17113CIC9NINV</t>
+  </si>
+  <si>
+    <t>BL17113CID3NINV</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>08156529333</t>
+  </si>
+  <si>
+    <t>BL171111TJYDELC</t>
+  </si>
+  <si>
+    <t>BL171111TKUNELC</t>
+  </si>
+  <si>
+    <t>BL17113CRO78INV</t>
+  </si>
+  <si>
+    <t>BL171111TO88ELC</t>
+  </si>
+  <si>
+    <t>BL171111TSFDELC</t>
+  </si>
+  <si>
+    <t>BL17113CY1IIINV</t>
+  </si>
+  <si>
+    <t>082136753334</t>
+  </si>
+  <si>
+    <t>BL17113CY3C3INV</t>
+  </si>
+  <si>
+    <t>BL17113CY48NINV</t>
+  </si>
+  <si>
+    <t>BL171111TTI8ELC</t>
+  </si>
+  <si>
+    <t>BL17113CZEVDINV</t>
+  </si>
+  <si>
+    <t>Ummu Uswah</t>
+  </si>
+  <si>
+    <t>085759049986</t>
+  </si>
+  <si>
+    <t>BL17113D59EDINV</t>
+  </si>
+  <si>
+    <t>085353845443</t>
+  </si>
+  <si>
+    <t>BL171111U3J8ELC</t>
+  </si>
+  <si>
+    <t>521080685472/45004248022</t>
+  </si>
+  <si>
+    <t>SUMARSONO PS</t>
+  </si>
+  <si>
+    <t>BL171111U6PIELC</t>
+  </si>
+  <si>
+    <t>BL171111U6QNELC</t>
+  </si>
+  <si>
+    <t>BL17113DCIXSINV</t>
+  </si>
+  <si>
+    <t>BL17113DFIZSINV</t>
+  </si>
+  <si>
+    <t>BL17113DGJA3INV</t>
+  </si>
+  <si>
+    <t>BL171111UJXSELC</t>
+  </si>
+  <si>
+    <t>Agus Proof</t>
+  </si>
+  <si>
+    <t>524030043045</t>
+  </si>
+  <si>
+    <t>IMAN MUHADI</t>
+  </si>
+  <si>
+    <t>BL17113DIZLNINV</t>
+  </si>
+  <si>
+    <t>BL171111UK63ELC</t>
+  </si>
+  <si>
+    <t>BL17113DKEL3INV</t>
+  </si>
+  <si>
+    <t>085228250800</t>
+  </si>
+  <si>
+    <t>BL17113D9OBDINV</t>
+  </si>
+  <si>
+    <t>Mbak Maya</t>
+  </si>
+  <si>
+    <t>085878565650</t>
   </si>
   <si>
     <t>NO TRANSAKSI</t>
@@ -1496,12 +1616,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1559,7 +1679,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1573,8 +1693,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1588,11 +1730,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1604,14 +1760,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -1620,11 +1768,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1651,14 +1799,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -1666,43 +1806,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1717,49 +1837,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFAFAFA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1777,7 +1855,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1789,7 +1939,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1801,13 +1969,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1819,49 +2011,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1873,36 +2023,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1963,6 +2089,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFEEEEEE"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1974,6 +2109,26 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2040,34 +2195,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2079,134 +2214,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2229,8 +2364,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2240,7 +2375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2251,7 +2386,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2264,13 +2399,13 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2296,8 +2431,16 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -2352,6 +2495,11 @@
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2640,12 +2788,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:N289"/>
+  <dimension ref="A1:N368"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A243" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A273" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I266" sqref="I266"/>
+      <selection pane="bottomLeft" activeCell="A296" sqref="A296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5178,7 +5326,6 @@
       <c r="D79" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="E79" s="25"/>
       <c r="F79" s="34">
         <v>11000</v>
       </c>
@@ -6968,7 +7115,7 @@
       </c>
     </row>
     <row r="130" spans="1:11">
-      <c r="A130" s="52" t="s">
+      <c r="A130" s="55" t="s">
         <v>239</v>
       </c>
       <c r="B130" s="33">
@@ -7005,7 +7152,7 @@
       </c>
     </row>
     <row r="131" spans="1:11">
-      <c r="A131" s="52" t="s">
+      <c r="A131" s="55" t="s">
         <v>241</v>
       </c>
       <c r="B131" s="33">
@@ -7040,7 +7187,7 @@
       </c>
     </row>
     <row r="132" spans="1:11">
-      <c r="A132" s="52" t="s">
+      <c r="A132" s="55" t="s">
         <v>244</v>
       </c>
       <c r="B132" s="33">
@@ -7077,7 +7224,7 @@
       </c>
     </row>
     <row r="133" spans="1:11">
-      <c r="A133" s="52" t="s">
+      <c r="A133" s="55" t="s">
         <v>246</v>
       </c>
       <c r="B133" s="33">
@@ -7151,7 +7298,7 @@
       </c>
     </row>
     <row r="135" spans="1:11">
-      <c r="A135" s="52" t="s">
+      <c r="A135" s="55" t="s">
         <v>252</v>
       </c>
       <c r="B135" s="33">
@@ -7188,7 +7335,7 @@
       </c>
     </row>
     <row r="136" spans="1:11">
-      <c r="A136" s="52" t="s">
+      <c r="A136" s="55" t="s">
         <v>253</v>
       </c>
       <c r="B136" s="33">
@@ -7225,7 +7372,7 @@
       </c>
     </row>
     <row r="137" spans="1:11">
-      <c r="A137" s="52" t="s">
+      <c r="A137" s="55" t="s">
         <v>256</v>
       </c>
       <c r="B137" s="33">
@@ -7262,7 +7409,7 @@
       </c>
     </row>
     <row r="138" spans="1:11">
-      <c r="A138" s="52" t="s">
+      <c r="A138" s="55" t="s">
         <v>258</v>
       </c>
       <c r="B138" s="33">
@@ -7296,7 +7443,7 @@
       </c>
     </row>
     <row r="139" spans="1:11">
-      <c r="A139" s="52" t="s">
+      <c r="A139" s="55" t="s">
         <v>259</v>
       </c>
       <c r="B139" s="33">
@@ -7555,7 +7702,7 @@
       </c>
     </row>
     <row r="146" spans="1:11">
-      <c r="A146" s="52" t="s">
+      <c r="A146" s="55" t="s">
         <v>270</v>
       </c>
       <c r="B146" s="33">
@@ -7589,7 +7736,7 @@
       </c>
     </row>
     <row r="147" spans="1:11">
-      <c r="A147" s="52" t="s">
+      <c r="A147" s="55" t="s">
         <v>273</v>
       </c>
       <c r="B147" s="33">
@@ -7623,7 +7770,7 @@
       </c>
     </row>
     <row r="148" spans="1:11">
-      <c r="A148" s="52" t="s">
+      <c r="A148" s="55" t="s">
         <v>275</v>
       </c>
       <c r="B148" s="33">
@@ -7657,7 +7804,7 @@
       </c>
     </row>
     <row r="149" spans="1:11">
-      <c r="A149" s="52" t="s">
+      <c r="A149" s="55" t="s">
         <v>277</v>
       </c>
       <c r="B149" s="33">
@@ -7691,7 +7838,7 @@
       </c>
     </row>
     <row r="150" spans="1:11">
-      <c r="A150" s="52" t="s">
+      <c r="A150" s="55" t="s">
         <v>279</v>
       </c>
       <c r="B150" s="33">
@@ -7722,7 +7869,7 @@
       </c>
     </row>
     <row r="151" spans="1:11">
-      <c r="A151" s="52" t="s">
+      <c r="A151" s="55" t="s">
         <v>280</v>
       </c>
       <c r="B151" s="33">
@@ -7793,7 +7940,7 @@
       </c>
     </row>
     <row r="153" spans="1:11">
-      <c r="A153" s="52" t="s">
+      <c r="A153" s="55" t="s">
         <v>286</v>
       </c>
       <c r="B153" s="33">
@@ -7827,7 +7974,7 @@
       </c>
     </row>
     <row r="154" spans="1:11">
-      <c r="A154" s="52" t="s">
+      <c r="A154" s="55" t="s">
         <v>287</v>
       </c>
       <c r="B154" s="33">
@@ -7898,7 +8045,7 @@
       </c>
     </row>
     <row r="156" spans="1:11">
-      <c r="A156" s="52" t="s">
+      <c r="A156" s="55" t="s">
         <v>292</v>
       </c>
       <c r="B156" s="33">
@@ -7969,7 +8116,7 @@
       </c>
     </row>
     <row r="158" spans="1:11">
-      <c r="A158" s="52" t="s">
+      <c r="A158" s="55" t="s">
         <v>295</v>
       </c>
       <c r="B158" s="33">
@@ -8040,7 +8187,7 @@
       </c>
     </row>
     <row r="160" spans="1:11">
-      <c r="A160" s="52" t="s">
+      <c r="A160" s="55" t="s">
         <v>297</v>
       </c>
       <c r="B160" s="33">
@@ -8111,7 +8258,7 @@
       </c>
     </row>
     <row r="162" spans="1:11">
-      <c r="A162" s="52" t="s">
+      <c r="A162" s="55" t="s">
         <v>301</v>
       </c>
       <c r="B162" s="33">
@@ -8145,7 +8292,7 @@
       </c>
     </row>
     <row r="163" spans="1:11">
-      <c r="A163" s="52" t="s">
+      <c r="A163" s="55" t="s">
         <v>302</v>
       </c>
       <c r="B163" s="33">
@@ -8179,7 +8326,7 @@
       </c>
     </row>
     <row r="164" spans="1:11">
-      <c r="A164" s="52" t="s">
+      <c r="A164" s="55" t="s">
         <v>303</v>
       </c>
       <c r="B164" s="33">
@@ -8210,7 +8357,7 @@
       </c>
     </row>
     <row r="165" spans="1:11">
-      <c r="A165" s="52" t="s">
+      <c r="A165" s="55" t="s">
         <v>306</v>
       </c>
       <c r="B165" s="33">
@@ -8244,7 +8391,7 @@
       </c>
     </row>
     <row r="166" spans="1:11">
-      <c r="A166" s="52" t="s">
+      <c r="A166" s="55" t="s">
         <v>307</v>
       </c>
       <c r="B166" s="33">
@@ -8278,7 +8425,7 @@
       </c>
     </row>
     <row r="167" spans="1:11">
-      <c r="A167" s="52" t="s">
+      <c r="A167" s="55" t="s">
         <v>310</v>
       </c>
       <c r="B167" s="33">
@@ -8442,7 +8589,7 @@
       </c>
     </row>
     <row r="172" spans="1:11">
-      <c r="A172" s="52" t="s">
+      <c r="A172" s="55" t="s">
         <v>318</v>
       </c>
       <c r="B172" s="33">
@@ -9494,7 +9641,7 @@
       <c r="C201" t="s">
         <v>97</v>
       </c>
-      <c r="D201" s="53" t="s">
+      <c r="D201" s="56" t="s">
         <v>361</v>
       </c>
       <c r="F201" s="26">
@@ -10195,6 +10342,9 @@
       <c r="H221" s="26">
         <v>101500</v>
       </c>
+      <c r="I221" s="26">
+        <v>100000</v>
+      </c>
       <c r="J221" s="38">
         <f t="shared" si="8"/>
         <v>5075</v>
@@ -10891,7 +11041,7 @@
       <c r="C242" t="s">
         <v>438</v>
       </c>
-      <c r="D242" s="53" t="s">
+      <c r="D242" s="56" t="s">
         <v>361</v>
       </c>
       <c r="F242" s="26">
@@ -11627,7 +11777,7 @@
       </c>
     </row>
     <row r="264" spans="1:11">
-      <c r="A264" s="51" t="s">
+      <c r="A264" s="49" t="s">
         <v>467</v>
       </c>
       <c r="B264" s="33">
@@ -11639,7 +11789,6 @@
       <c r="D264" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="E264" s="25"/>
       <c r="F264" s="34">
         <v>11300</v>
       </c>
@@ -11661,261 +11810,1810 @@
         <v>565</v>
       </c>
     </row>
-    <row r="265" spans="2:11">
+    <row r="265" ht="30" spans="1:11">
+      <c r="A265" s="49" t="s">
+        <v>468</v>
+      </c>
       <c r="B265" s="33">
-        <v>42883</v>
+        <v>42884</v>
+      </c>
+      <c r="C265" t="s">
+        <v>399</v>
+      </c>
+      <c r="D265" s="24" t="s">
+        <v>400</v>
+      </c>
+      <c r="E265" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="F265" s="26">
+        <v>100000</v>
+      </c>
+      <c r="G265" t="s">
+        <v>16</v>
+      </c>
+      <c r="H265" s="26">
+        <v>101500</v>
+      </c>
+      <c r="I265" s="26">
+        <v>100000</v>
       </c>
       <c r="J265" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5075</v>
       </c>
       <c r="K265" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="266" spans="10:11">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="266" spans="1:11">
+      <c r="A266" s="49" t="s">
+        <v>469</v>
+      </c>
+      <c r="B266" s="33">
+        <v>42884</v>
+      </c>
+      <c r="C266" t="s">
+        <v>210</v>
+      </c>
+      <c r="D266" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="F266" s="26">
+        <v>59000</v>
+      </c>
+      <c r="G266" t="s">
+        <v>212</v>
+      </c>
+      <c r="H266" s="26">
+        <v>58000</v>
+      </c>
       <c r="J266" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2900</v>
       </c>
       <c r="K266" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="267" spans="10:11">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="267" spans="1:11">
+      <c r="A267" s="49" t="s">
+        <v>470</v>
+      </c>
+      <c r="B267" s="33">
+        <v>42884</v>
+      </c>
+      <c r="C267" t="s">
+        <v>72</v>
+      </c>
+      <c r="D267" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F267" s="26">
+        <v>50000</v>
+      </c>
+      <c r="G267" t="s">
+        <v>12</v>
+      </c>
+      <c r="H267" s="26">
+        <v>49500</v>
+      </c>
+      <c r="I267" s="26">
+        <v>50000</v>
+      </c>
       <c r="J267" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2475</v>
       </c>
       <c r="K267" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="268" spans="10:11">
+        <v>2975</v>
+      </c>
+    </row>
+    <row r="268" spans="1:11">
+      <c r="A268" s="51" t="s">
+        <v>471</v>
+      </c>
+      <c r="B268" s="33">
+        <v>42884</v>
+      </c>
+      <c r="C268" t="s">
+        <v>472</v>
+      </c>
+      <c r="D268" s="24" t="s">
+        <v>473</v>
+      </c>
+      <c r="F268" s="26">
+        <v>26000</v>
+      </c>
+      <c r="G268" t="s">
+        <v>12</v>
+      </c>
+      <c r="H268" s="26">
+        <v>25000</v>
+      </c>
       <c r="J268" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1250</v>
       </c>
       <c r="K268" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="269" spans="10:11">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="269" spans="1:11">
+      <c r="A269" s="49" t="s">
+        <v>474</v>
+      </c>
+      <c r="B269" s="33">
+        <v>42884</v>
+      </c>
+      <c r="C269" t="s">
+        <v>130</v>
+      </c>
+      <c r="D269" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="F269" s="26">
+        <v>100000</v>
+      </c>
+      <c r="G269" t="s">
+        <v>16</v>
+      </c>
+      <c r="H269" s="26">
+        <v>101500</v>
+      </c>
       <c r="J269" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5075</v>
       </c>
       <c r="K269" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="270" spans="10:11">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="270" spans="1:11">
+      <c r="A270" s="49" t="s">
+        <v>475</v>
+      </c>
+      <c r="B270" s="33">
+        <v>42884</v>
+      </c>
+      <c r="C270" t="s">
+        <v>472</v>
+      </c>
+      <c r="D270" s="45" t="s">
+        <v>196</v>
+      </c>
+      <c r="F270" s="26">
+        <v>51000</v>
+      </c>
+      <c r="G270" t="s">
+        <v>16</v>
+      </c>
+      <c r="H270" s="26">
+        <v>51500</v>
+      </c>
       <c r="J270" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2575</v>
       </c>
       <c r="K270" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="271" spans="10:11">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="271" spans="1:11">
+      <c r="A271" s="49" t="s">
+        <v>476</v>
+      </c>
+      <c r="B271" s="33">
+        <v>42884</v>
+      </c>
+      <c r="C271" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="D271" s="41" t="s">
+        <v>231</v>
+      </c>
+      <c r="F271" s="26">
+        <v>12000</v>
+      </c>
+      <c r="G271" t="s">
+        <v>12</v>
+      </c>
+      <c r="H271" s="26">
+        <v>10300</v>
+      </c>
+      <c r="I271" s="26">
+        <v>12000</v>
+      </c>
       <c r="J271" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>515</v>
       </c>
       <c r="K271" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="272" spans="10:11">
+        <v>2215</v>
+      </c>
+    </row>
+    <row r="272" spans="1:11">
+      <c r="A272" s="49" t="s">
+        <v>477</v>
+      </c>
+      <c r="B272" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C272" t="s">
+        <v>81</v>
+      </c>
+      <c r="D272" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E272" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F272" s="26">
+        <v>50000</v>
+      </c>
+      <c r="G272" t="s">
+        <v>16</v>
+      </c>
+      <c r="H272" s="26">
+        <v>51500</v>
+      </c>
+      <c r="I272" s="34">
+        <v>51000</v>
+      </c>
       <c r="J272" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2575</v>
       </c>
       <c r="K272" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="273" spans="10:11">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="273" spans="1:11">
+      <c r="A273" s="50" t="s">
+        <v>478</v>
+      </c>
+      <c r="B273" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C273" t="s">
+        <v>138</v>
+      </c>
+      <c r="D273" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="E273" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="F273" s="34">
+        <v>51500</v>
+      </c>
+      <c r="G273" t="s">
+        <v>16</v>
+      </c>
+      <c r="H273" s="34">
+        <v>50000</v>
+      </c>
+      <c r="I273" s="34">
+        <v>51500</v>
+      </c>
       <c r="J273" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="K273" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="274" spans="10:11">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="274" spans="1:11">
+      <c r="A274" s="49" t="s">
+        <v>479</v>
+      </c>
+      <c r="B274" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C274" t="s">
+        <v>472</v>
+      </c>
+      <c r="D274" s="24" t="s">
+        <v>480</v>
+      </c>
+      <c r="F274" s="26">
+        <v>12000</v>
+      </c>
+      <c r="G274" t="s">
+        <v>12</v>
+      </c>
+      <c r="H274" s="26">
+        <v>11300</v>
+      </c>
       <c r="J274" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>565</v>
       </c>
       <c r="K274" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="275" spans="10:11">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11">
+      <c r="A275" s="50" t="s">
+        <v>481</v>
+      </c>
+      <c r="B275" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C275" t="s">
+        <v>308</v>
+      </c>
+      <c r="D275" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="E275" s="25" t="s">
+        <v>308</v>
+      </c>
+      <c r="F275" s="26">
+        <v>12000</v>
+      </c>
+      <c r="G275" t="s">
+        <v>12</v>
+      </c>
+      <c r="H275" s="26">
+        <v>11300</v>
+      </c>
       <c r="J275" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>565</v>
       </c>
       <c r="K275" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="276" spans="10:11">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="276" spans="1:11">
+      <c r="A276" s="50" t="s">
+        <v>482</v>
+      </c>
+      <c r="B276" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C276" t="s">
+        <v>24</v>
+      </c>
+      <c r="D276" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="E276" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="F276" s="26">
+        <v>12000</v>
+      </c>
+      <c r="G276" t="s">
+        <v>12</v>
+      </c>
+      <c r="H276" s="26">
+        <v>11300</v>
+      </c>
       <c r="J276" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>565</v>
       </c>
       <c r="K276" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="277" spans="10:11">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="277" spans="1:11">
+      <c r="A277" s="49" t="s">
+        <v>483</v>
+      </c>
+      <c r="B277" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C277" t="s">
+        <v>90</v>
+      </c>
+      <c r="D277" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E277" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F277" s="26">
+        <v>21500</v>
+      </c>
+      <c r="G277" t="s">
+        <v>12</v>
+      </c>
+      <c r="H277" s="26">
+        <v>21500</v>
+      </c>
       <c r="J277" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1075</v>
       </c>
       <c r="K277" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="278" spans="10:11">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="278" spans="1:11">
+      <c r="A278" s="49" t="s">
+        <v>484</v>
+      </c>
+      <c r="B278" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C278" t="s">
+        <v>485</v>
+      </c>
+      <c r="D278" s="24" t="s">
+        <v>486</v>
+      </c>
+      <c r="F278" s="26">
+        <v>12000</v>
+      </c>
+      <c r="G278" t="s">
+        <v>12</v>
+      </c>
+      <c r="H278" s="26">
+        <v>11300</v>
+      </c>
       <c r="J278" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>565</v>
       </c>
       <c r="K278" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="279" spans="10:11">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="279" spans="1:11">
+      <c r="A279" s="49" t="s">
+        <v>487</v>
+      </c>
+      <c r="B279" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C279" t="s">
+        <v>308</v>
+      </c>
+      <c r="D279" s="24" t="s">
+        <v>488</v>
+      </c>
+      <c r="F279" s="26">
+        <v>12000</v>
+      </c>
+      <c r="G279" t="s">
+        <v>12</v>
+      </c>
+      <c r="H279" s="26">
+        <v>11300</v>
+      </c>
       <c r="J279" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>565</v>
       </c>
       <c r="K279" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="280" spans="10:11">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11">
+      <c r="A280" s="49" t="s">
+        <v>489</v>
+      </c>
+      <c r="B280" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C280" t="s">
+        <v>472</v>
+      </c>
+      <c r="D280" s="24" t="s">
+        <v>490</v>
+      </c>
+      <c r="E280" s="25" t="s">
+        <v>491</v>
+      </c>
+      <c r="F280" s="26">
+        <v>51000</v>
+      </c>
+      <c r="G280" t="s">
+        <v>16</v>
+      </c>
+      <c r="H280" s="26">
+        <v>51500</v>
+      </c>
       <c r="J280" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2575</v>
       </c>
       <c r="K280" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="281" spans="10:11">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="281" spans="1:11">
+      <c r="A281" s="49" t="s">
+        <v>492</v>
+      </c>
+      <c r="B281" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C281" t="s">
+        <v>9</v>
+      </c>
+      <c r="D281" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E281" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F281" s="26">
+        <v>100000</v>
+      </c>
+      <c r="G281" t="s">
+        <v>16</v>
+      </c>
+      <c r="H281" s="26">
+        <v>101500</v>
+      </c>
       <c r="J281" s="38">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5075</v>
       </c>
       <c r="K281" s="26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="282" spans="10:11">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="282" spans="1:11">
+      <c r="A282" s="49" t="s">
+        <v>493</v>
+      </c>
+      <c r="B282" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C282" t="s">
+        <v>390</v>
+      </c>
+      <c r="D282" s="24" t="s">
+        <v>391</v>
+      </c>
+      <c r="E282" s="25" t="s">
+        <v>392</v>
+      </c>
+      <c r="F282" s="26">
+        <v>100000</v>
+      </c>
+      <c r="G282" t="s">
+        <v>16</v>
+      </c>
+      <c r="H282" s="26">
+        <v>101500</v>
+      </c>
+      <c r="I282" s="26">
+        <v>100000</v>
+      </c>
       <c r="J282" s="38">
-        <f t="shared" ref="J282:J289" si="10">H282*5%</f>
-        <v>0</v>
+        <f t="shared" ref="J282:J345" si="10">H282*5%</f>
+        <v>5075</v>
       </c>
       <c r="K282" s="26">
-        <f t="shared" ref="K282:K289" si="11">J282-(H282-F282)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="283" spans="10:11">
+        <f t="shared" ref="K282:K345" si="11">J282-(H282-F282)</f>
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11">
+      <c r="A283" s="50" t="s">
+        <v>494</v>
+      </c>
+      <c r="B283" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C283" t="s">
+        <v>11</v>
+      </c>
+      <c r="D283" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="F283" s="26">
+        <v>12000</v>
+      </c>
+      <c r="G283" t="s">
+        <v>12</v>
+      </c>
+      <c r="H283" s="26">
+        <v>11300</v>
+      </c>
       <c r="J283" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>565</v>
       </c>
       <c r="K283" s="26">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="284" spans="10:11">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="284" spans="1:11">
+      <c r="A284" s="49" t="s">
+        <v>495</v>
+      </c>
+      <c r="B284" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C284" t="s">
+        <v>249</v>
+      </c>
+      <c r="D284" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="F284" s="26">
+        <v>34500</v>
+      </c>
+      <c r="G284" t="s">
+        <v>10</v>
+      </c>
+      <c r="H284" s="26">
+        <v>33500</v>
+      </c>
       <c r="J284" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1675</v>
       </c>
       <c r="K284" s="26">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="285" spans="10:11">
+        <v>2675</v>
+      </c>
+    </row>
+    <row r="285" ht="15.75" spans="1:11">
+      <c r="A285" s="49" t="s">
+        <v>496</v>
+      </c>
+      <c r="B285" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C285" t="s">
+        <v>120</v>
+      </c>
+      <c r="D285" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="F285" s="26">
+        <v>50000</v>
+      </c>
+      <c r="G285" t="s">
+        <v>16</v>
+      </c>
+      <c r="H285" s="26">
+        <v>51200</v>
+      </c>
       <c r="J285" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>2560</v>
       </c>
       <c r="K285" s="26">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="286" spans="10:11">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="286" spans="1:11">
+      <c r="A286" s="49" t="s">
+        <v>497</v>
+      </c>
+      <c r="B286" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C286" t="s">
+        <v>498</v>
+      </c>
+      <c r="D286" s="24" t="s">
+        <v>499</v>
+      </c>
+      <c r="E286" s="52" t="s">
+        <v>500</v>
+      </c>
+      <c r="F286" s="26">
+        <v>100000</v>
+      </c>
+      <c r="G286" t="s">
+        <v>16</v>
+      </c>
+      <c r="H286" s="26">
+        <v>101500</v>
+      </c>
       <c r="J286" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5075</v>
       </c>
       <c r="K286" s="26">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="287" spans="10:11">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="287" spans="1:11">
+      <c r="A287" s="50" t="s">
+        <v>501</v>
+      </c>
+      <c r="B287" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C287" t="s">
+        <v>120</v>
+      </c>
+      <c r="D287" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="F287" s="26">
+        <v>25000</v>
+      </c>
+      <c r="G287" t="s">
+        <v>12</v>
+      </c>
+      <c r="H287" s="26">
+        <v>25500</v>
+      </c>
       <c r="J287" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1275</v>
       </c>
       <c r="K287" s="26">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="288" spans="10:11">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="288" spans="1:11">
+      <c r="A288" s="50" t="s">
+        <v>502</v>
+      </c>
+      <c r="B288" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C288" t="s">
+        <v>142</v>
+      </c>
+      <c r="D288" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="E288" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="F288" s="34">
+        <v>20500</v>
+      </c>
+      <c r="G288" t="s">
+        <v>16</v>
+      </c>
+      <c r="H288" s="34">
+        <v>20500</v>
+      </c>
       <c r="J288" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1025</v>
       </c>
       <c r="K288" s="26">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="289" spans="10:11">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="289" spans="1:11">
+      <c r="A289" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="B289" s="33">
+        <v>42885</v>
+      </c>
+      <c r="C289" t="s">
+        <v>355</v>
+      </c>
+      <c r="D289" s="24" t="s">
+        <v>504</v>
+      </c>
+      <c r="F289" s="26">
+        <v>100000</v>
+      </c>
+      <c r="G289" t="s">
+        <v>16</v>
+      </c>
+      <c r="H289" s="26">
+        <v>98500</v>
+      </c>
+      <c r="I289" s="26">
+        <v>100000</v>
+      </c>
       <c r="J289" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4925</v>
       </c>
       <c r="K289" s="26">
         <f t="shared" si="11"/>
+        <v>6425</v>
+      </c>
+    </row>
+    <row r="290" spans="1:11">
+      <c r="A290" s="53" t="s">
+        <v>505</v>
+      </c>
+      <c r="B290" s="33">
+        <v>42886</v>
+      </c>
+      <c r="C290" t="s">
+        <v>506</v>
+      </c>
+      <c r="D290" s="24" t="s">
+        <v>507</v>
+      </c>
+      <c r="E290" s="25" t="s">
+        <v>506</v>
+      </c>
+      <c r="F290" s="26">
+        <v>197500</v>
+      </c>
+      <c r="G290" t="s">
+        <v>12</v>
+      </c>
+      <c r="H290" s="26">
+        <v>195000</v>
+      </c>
+      <c r="I290" s="26">
+        <v>197500</v>
+      </c>
+      <c r="J290" s="38">
+        <f t="shared" si="10"/>
+        <v>9750</v>
+      </c>
+      <c r="K290" s="26">
+        <f t="shared" si="11"/>
+        <v>12250</v>
+      </c>
+    </row>
+    <row r="291" spans="1:11">
+      <c r="A291" s="53" t="s">
+        <v>494</v>
+      </c>
+      <c r="B291" s="33">
+        <v>42886</v>
+      </c>
+      <c r="C291" t="s">
+        <v>11</v>
+      </c>
+      <c r="D291" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="E291" t="s">
+        <v>11</v>
+      </c>
+      <c r="F291" s="26">
+        <v>12000</v>
+      </c>
+      <c r="G291" t="s">
+        <v>12</v>
+      </c>
+      <c r="H291" s="26">
+        <v>11300</v>
+      </c>
+      <c r="I291" s="26">
+        <v>12000</v>
+      </c>
+      <c r="J291" s="38">
+        <f t="shared" si="10"/>
+        <v>565</v>
+      </c>
+      <c r="K291" s="26">
+        <f t="shared" si="11"/>
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="292" spans="1:11">
+      <c r="A292" s="53" t="s">
+        <v>495</v>
+      </c>
+      <c r="B292" s="33">
+        <v>42886</v>
+      </c>
+      <c r="C292" t="s">
+        <v>249</v>
+      </c>
+      <c r="D292" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="F292" s="26">
+        <v>34500</v>
+      </c>
+      <c r="G292" t="s">
+        <v>10</v>
+      </c>
+      <c r="H292" s="26">
+        <v>33500</v>
+      </c>
+      <c r="J292" s="38">
+        <f t="shared" si="10"/>
+        <v>1675</v>
+      </c>
+      <c r="K292" s="26">
+        <f t="shared" si="11"/>
+        <v>2675</v>
+      </c>
+    </row>
+    <row r="293" ht="15.75" spans="1:11">
+      <c r="A293" s="53" t="s">
+        <v>496</v>
+      </c>
+      <c r="B293" s="33">
+        <v>42886</v>
+      </c>
+      <c r="C293" t="s">
+        <v>120</v>
+      </c>
+      <c r="D293" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="F293" s="34">
+        <v>50000</v>
+      </c>
+      <c r="G293" t="s">
+        <v>12</v>
+      </c>
+      <c r="H293" s="26">
+        <v>51200</v>
+      </c>
+      <c r="I293" s="34">
+        <v>48000</v>
+      </c>
+      <c r="J293" s="38">
+        <f t="shared" si="10"/>
+        <v>2560</v>
+      </c>
+      <c r="K293" s="26">
+        <f t="shared" si="11"/>
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="294" spans="1:11">
+      <c r="A294" s="53" t="s">
+        <v>497</v>
+      </c>
+      <c r="B294" s="33">
+        <v>42886</v>
+      </c>
+      <c r="C294" t="s">
+        <v>498</v>
+      </c>
+      <c r="D294" s="24" t="s">
+        <v>499</v>
+      </c>
+      <c r="E294" s="52" t="s">
+        <v>500</v>
+      </c>
+      <c r="F294" s="26">
+        <v>100000</v>
+      </c>
+      <c r="G294" t="s">
+        <v>16</v>
+      </c>
+      <c r="H294" s="26">
+        <v>101500</v>
+      </c>
+      <c r="J294" s="38">
+        <f t="shared" si="10"/>
+        <v>5075</v>
+      </c>
+      <c r="K294" s="26">
+        <f t="shared" si="11"/>
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="295" spans="1:11">
+      <c r="A295" s="53" t="s">
+        <v>501</v>
+      </c>
+      <c r="B295" s="33">
+        <v>42886</v>
+      </c>
+      <c r="C295" t="s">
+        <v>120</v>
+      </c>
+      <c r="D295" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="F295" s="26">
+        <v>25000</v>
+      </c>
+      <c r="G295" t="s">
+        <v>12</v>
+      </c>
+      <c r="H295" s="26">
+        <v>25500</v>
+      </c>
+      <c r="J295" s="38">
+        <f t="shared" si="10"/>
+        <v>1275</v>
+      </c>
+      <c r="K295" s="26">
+        <f t="shared" si="11"/>
+        <v>775</v>
+      </c>
+    </row>
+    <row r="296" spans="2:11">
+      <c r="B296" s="33">
+        <v>42886</v>
+      </c>
+      <c r="J296" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K296" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="2:11">
+      <c r="B297" s="33">
+        <v>42886</v>
+      </c>
+      <c r="J297" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K297" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="2:11">
+      <c r="B298" s="33">
+        <v>42886</v>
+      </c>
+      <c r="J298" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K298" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="2:11">
+      <c r="B299" s="33">
+        <v>42886</v>
+      </c>
+      <c r="J299" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K299" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="2:11">
+      <c r="B300" s="33">
+        <v>42886</v>
+      </c>
+      <c r="J300" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K300" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="2:11">
+      <c r="B301" s="33">
+        <v>42886</v>
+      </c>
+      <c r="J301" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K301" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="2:11">
+      <c r="B302" s="33">
+        <v>42886</v>
+      </c>
+      <c r="J302" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K302" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="2:11">
+      <c r="B303" s="33">
+        <v>42886</v>
+      </c>
+      <c r="J303" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K303" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="2:11">
+      <c r="B304" s="33">
+        <v>42886</v>
+      </c>
+      <c r="J304" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K304" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="2:11">
+      <c r="B305" s="33">
+        <v>42886</v>
+      </c>
+      <c r="J305" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K305" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="2:11">
+      <c r="B306" s="33">
+        <v>42886</v>
+      </c>
+      <c r="J306" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K306" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="2:11">
+      <c r="B307" s="33">
+        <v>42886</v>
+      </c>
+      <c r="J307" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K307" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="2:11">
+      <c r="B308" s="33">
+        <v>42886</v>
+      </c>
+      <c r="J308" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K308" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="10:11">
+      <c r="J309" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K309" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="10:11">
+      <c r="J310" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K310" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="10:11">
+      <c r="J311" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K311" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="10:11">
+      <c r="J312" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K312" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="10:11">
+      <c r="J313" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K313" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="10:11">
+      <c r="J314" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K314" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="10:11">
+      <c r="J315" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K315" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="10:11">
+      <c r="J316" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K316" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="10:11">
+      <c r="J317" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K317" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="10:11">
+      <c r="J318" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K318" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="10:11">
+      <c r="J319" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K319" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="10:11">
+      <c r="J320" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K320" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="10:11">
+      <c r="J321" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K321" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="10:11">
+      <c r="J322" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K322" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="10:11">
+      <c r="J323" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K323" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="10:11">
+      <c r="J324" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K324" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="10:11">
+      <c r="J325" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K325" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="10:11">
+      <c r="J326" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K326" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="10:11">
+      <c r="J327" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K327" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="10:11">
+      <c r="J328" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K328" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="10:11">
+      <c r="J329" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K329" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="10:11">
+      <c r="J330" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K330" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="10:11">
+      <c r="J331" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K331" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="10:11">
+      <c r="J332" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K332" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="10:11">
+      <c r="J333" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K333" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="10:11">
+      <c r="J334" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K334" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="10:11">
+      <c r="J335" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K335" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="10:11">
+      <c r="J336" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K336" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="10:11">
+      <c r="J337" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K337" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="10:11">
+      <c r="J338" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K338" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="10:11">
+      <c r="J339" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K339" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="10:11">
+      <c r="J340" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K340" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="10:11">
+      <c r="J341" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K341" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="10:11">
+      <c r="J342" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K342" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="10:11">
+      <c r="J343" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K343" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="10:11">
+      <c r="J344" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K344" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="345" spans="10:11">
+      <c r="J345" s="38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K345" s="26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="10:11">
+      <c r="J346" s="38">
+        <f t="shared" ref="J346:J368" si="12">H346*5%</f>
+        <v>0</v>
+      </c>
+      <c r="K346" s="26">
+        <f t="shared" ref="K346:K368" si="13">J346-(H346-F346)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="347" spans="10:11">
+      <c r="J347" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K347" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348" spans="10:11">
+      <c r="J348" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K348" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="349" spans="10:11">
+      <c r="J349" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K349" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350" spans="10:11">
+      <c r="J350" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K350" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="351" spans="10:11">
+      <c r="J351" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K351" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="352" spans="10:11">
+      <c r="J352" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K352" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="353" spans="10:11">
+      <c r="J353" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K353" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="10:11">
+      <c r="J354" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K354" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="355" spans="10:11">
+      <c r="J355" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K355" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356" spans="10:11">
+      <c r="J356" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K356" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="357" spans="10:11">
+      <c r="J357" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K357" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="358" spans="10:11">
+      <c r="J358" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K358" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="359" spans="10:11">
+      <c r="J359" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K359" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="360" spans="10:11">
+      <c r="J360" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K360" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361" spans="10:11">
+      <c r="J361" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K361" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="362" spans="10:11">
+      <c r="J362" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K362" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="10:11">
+      <c r="J363" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K363" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="364" spans="10:11">
+      <c r="J364" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K364" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="10:11">
+      <c r="J365" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K365" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="10:11">
+      <c r="J366" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K366" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="367" spans="10:11">
+      <c r="J367" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K367" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="368" spans="10:11">
+      <c r="J368" s="38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K368" s="26">
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:I265"/>
+  <autoFilter ref="B1:I308"/>
   <hyperlinks>
     <hyperlink ref="A173" r:id="rId1" display="BL171111JKC7ELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/795416"/>
     <hyperlink ref="A174" r:id="rId2" display="BL171111JMU2ELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/798491"/>
@@ -11999,6 +13697,37 @@
     <hyperlink ref="A262" r:id="rId80" display="BL171111T1SSELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1201472"/>
     <hyperlink ref="A263" r:id="rId81" display="BL17113CAB83INV" tooltip="https://www.bukalapak.com/payment/invoices/121948997"/>
     <hyperlink ref="A264" r:id="rId82" display="BL17113CCQIXINV" tooltip="https://www.bukalapak.com/payment/invoices/122053502"/>
+    <hyperlink ref="A265" r:id="rId83" display="BL171111TBBIELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1213117"/>
+    <hyperlink ref="A266" r:id="rId84" display="BL17113CGXX3INV" tooltip="https://www.bukalapak.com/payment/invoices/122234072"/>
+    <hyperlink ref="A267" r:id="rId85" display="BL17113CIC9NINV" tooltip="https://www.bukalapak.com/payment/invoices/122293277"/>
+    <hyperlink ref="A268" r:id="rId86" display="BL17113CID3NINV" tooltip="https://www.bukalapak.com/payment/invoices/122294292"/>
+    <hyperlink ref="A269" r:id="rId87" display="BL171111TJYDELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1223717"/>
+    <hyperlink ref="A270" r:id="rId88" display="BL171111TKUNELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1224812"/>
+    <hyperlink ref="A271" r:id="rId89" display="BL17113CRO78INV" tooltip="https://www.bukalapak.com/payment/invoices/122693767"/>
+    <hyperlink ref="A273" r:id="rId90" display="BL171111TSFDELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1234077"/>
+    <hyperlink ref="A272" r:id="rId91" display="BL171111TO88ELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1228927"/>
+    <hyperlink ref="A274" r:id="rId92" display="BL17113CY1IIINV" tooltip="https://www.bukalapak.com/payment/invoices/122966112"/>
+    <hyperlink ref="A276" r:id="rId93" display="BL17113CY48NINV" tooltip="https://www.bukalapak.com/payment/invoices/122969442"/>
+    <hyperlink ref="A275" r:id="rId94" display="BL17113CY3C3INV" tooltip="https://www.bukalapak.com/payment/invoices/122968337"/>
+    <hyperlink ref="A277" r:id="rId95" display="BL171111TTI8ELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1235402"/>
+    <hyperlink ref="A278" r:id="rId96" display="BL17113CZEVDINV" tooltip="https://www.bukalapak.com/payment/invoices/123025362"/>
+    <hyperlink ref="A279" r:id="rId97" display="BL17113D59EDINV" tooltip="https://www.bukalapak.com/payment/invoices/123233017"/>
+    <hyperlink ref="A280" r:id="rId98" display="BL171111U3J8ELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1246462"/>
+    <hyperlink ref="A281" r:id="rId99" display="BL171111U6PIELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1250357"/>
+    <hyperlink ref="A282" r:id="rId100" display="BL171111U6QNELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1250397"/>
+    <hyperlink ref="A283" r:id="rId101" display="BL17113DCIXSINV" tooltip="https://www.bukalapak.com/payment/invoices/123544847"/>
+    <hyperlink ref="A284" r:id="rId102" display="BL17113DFIZSINV" tooltip="https://www.bukalapak.com/payment/invoices/123673542"/>
+    <hyperlink ref="A285" r:id="rId103" display="BL17113DGJA3INV" tooltip="https://www.bukalapak.com/payment/invoices/123716742"/>
+    <hyperlink ref="A286" r:id="rId104" display="BL171111UJXSELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1266572"/>
+    <hyperlink ref="A287" r:id="rId105" display="BL17113DIZLNINV" tooltip="https://www.bukalapak.com/payment/invoices/123822497"/>
+    <hyperlink ref="A288" r:id="rId106" display="BL171111UK63ELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1266827"/>
+    <hyperlink ref="A289" r:id="rId107" display="BL17113DKEL3INV" tooltip="https://www.bukalapak.com/payment/invoices/123882502"/>
+    <hyperlink ref="A290" r:id="rId108" display="BL17113D9OBDINV" tooltip="https://www.bukalapak.com/payment/invoices/123422787"/>
+    <hyperlink ref="A291" r:id="rId101" display="BL17113DCIXSINV" tooltip="https://www.bukalapak.com/payment/invoices/123544847"/>
+    <hyperlink ref="A292" r:id="rId102" display="BL17113DFIZSINV" tooltip="https://www.bukalapak.com/payment/invoices/123673542"/>
+    <hyperlink ref="A293" r:id="rId103" display="BL17113DGJA3INV" tooltip="https://www.bukalapak.com/payment/invoices/123716742"/>
+    <hyperlink ref="A294" r:id="rId104" display="BL171111UJXSELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1266572"/>
+    <hyperlink ref="A295" r:id="rId105" display="BL17113DIZLNINV" tooltip="https://www.bukalapak.com/payment/invoices/123822497"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -12026,19 +13755,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="20" t="s">
-        <v>468</v>
+        <v>508</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>469</v>
+        <v>509</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>470</v>
+        <v>510</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>471</v>
+        <v>511</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>472</v>
+        <v>512</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -12315,7 +14044,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
-        <v>473</v>
+        <v>513</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -12327,7 +14056,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="21" t="s">
-        <v>474</v>
+        <v>514</v>
       </c>
       <c r="E20" s="22">
         <f>5%*E18</f>
@@ -12336,7 +14065,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="21" t="s">
-        <v>475</v>
+        <v>515</v>
       </c>
       <c r="E21" s="22">
         <f>10%*E18</f>
@@ -12373,22 +14102,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>476</v>
+        <v>516</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>477</v>
+        <v>517</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>478</v>
+        <v>518</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>479</v>
+        <v>519</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -12467,7 +14196,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="7" t="s">
-        <v>480</v>
+        <v>520</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -12480,7 +14209,7 @@
     </row>
     <row r="9" spans="4:5">
       <c r="D9" s="11" t="s">
-        <v>481</v>
+        <v>521</v>
       </c>
       <c r="E9" s="12">
         <v>1000000</v>
@@ -12488,7 +14217,7 @@
     </row>
     <row r="10" spans="4:5">
       <c r="D10" s="13" t="s">
-        <v>482</v>
+        <v>522</v>
       </c>
       <c r="E10" s="5">
         <f>E9-E6</f>
@@ -12501,7 +14230,7 @@
     </row>
     <row r="12" spans="4:5">
       <c r="D12" s="3" t="s">
-        <v>483</v>
+        <v>523</v>
       </c>
       <c r="E12" s="5">
         <v>300000</v>
@@ -12509,7 +14238,7 @@
     </row>
     <row r="13" spans="4:5">
       <c r="D13" s="13" t="s">
-        <v>484</v>
+        <v>524</v>
       </c>
       <c r="E13" s="5">
         <v>300000</v>
@@ -12517,7 +14246,7 @@
     </row>
     <row r="14" spans="4:5">
       <c r="D14" s="11" t="s">
-        <v>485</v>
+        <v>525</v>
       </c>
       <c r="E14" s="12">
         <f>E13+E12</f>
@@ -12530,7 +14259,7 @@
     </row>
     <row r="16" spans="4:5">
       <c r="D16" s="11" t="s">
-        <v>486</v>
+        <v>526</v>
       </c>
       <c r="E16" s="12">
         <f>E10-E14</f>
@@ -12765,7 +14494,7 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="16" t="s">
-        <v>480</v>
+        <v>520</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -12778,7 +14507,7 @@
     </row>
     <row r="34" spans="4:5">
       <c r="D34" s="11" t="s">
-        <v>487</v>
+        <v>527</v>
       </c>
       <c r="E34" s="19">
         <f>E16</f>
@@ -12795,7 +14524,7 @@
     </row>
     <row r="36" spans="4:5">
       <c r="D36" s="11" t="s">
-        <v>488</v>
+        <v>528</v>
       </c>
       <c r="E36" s="19">
         <f>E34+E35</f>
@@ -12808,7 +14537,7 @@
     </row>
     <row r="38" spans="4:5">
       <c r="D38" s="11" t="s">
-        <v>489</v>
+        <v>529</v>
       </c>
       <c r="E38" s="19">
         <f>E36-E32</f>

</xml_diff>

<commit_message>
BL Juni Tgl 2 blm sls
</commit_message>
<xml_diff>
--- a/Jual Pulsa.xlsx
+++ b/Jual Pulsa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="19500" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539">
   <si>
     <t>No Transaksi</t>
   </si>
@@ -1543,6 +1543,33 @@
   </si>
   <si>
     <t>085878565650</t>
+  </si>
+  <si>
+    <t>BL17113DSL3NINV</t>
+  </si>
+  <si>
+    <t>085799241916</t>
+  </si>
+  <si>
+    <t>BL171111VECXELC</t>
+  </si>
+  <si>
+    <t>BL171111VPTXELC</t>
+  </si>
+  <si>
+    <t>BL17113EBDX8INV</t>
+  </si>
+  <si>
+    <t>BL171111W3C8ELC</t>
+  </si>
+  <si>
+    <t>BL17113EH6LNINV</t>
+  </si>
+  <si>
+    <t>BL17113EH7J8INV</t>
+  </si>
+  <si>
+    <t>085725221058</t>
   </si>
   <si>
     <t>NO TRANSAKSI</t>
@@ -1618,10 +1645,10 @@
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1678,8 +1705,30 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1694,15 +1743,30 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1716,22 +1780,55 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1746,77 +1843,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1843,108 +1870,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1957,7 +1882,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1969,7 +1912,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1981,7 +2014,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1993,37 +2044,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2115,10 +2142,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -2129,6 +2154,21 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2152,7 +2192,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2172,33 +2212,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2214,134 +2241,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2439,6 +2466,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
@@ -2495,11 +2523,6 @@
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -2791,25 +2814,25 @@
   <dimension ref="A1:N368"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A273" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A274" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A296" sqref="A296"/>
+      <selection pane="bottomLeft" activeCell="H305" sqref="H305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.7142857142857" style="23" customWidth="1"/>
-    <col min="2" max="2" width="9.71428571428571" customWidth="1"/>
+    <col min="1" max="1" width="22.7166666666667" style="23" customWidth="1"/>
+    <col min="2" max="2" width="9.71666666666667" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="25.2857142857143" style="24" customWidth="1"/>
-    <col min="5" max="5" width="27.5714285714286" style="25" customWidth="1"/>
-    <col min="6" max="6" width="11.5714285714286" style="26" customWidth="1"/>
-    <col min="7" max="7" width="11.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="25.2833333333333" style="24" customWidth="1"/>
+    <col min="5" max="5" width="27.575" style="25" customWidth="1"/>
+    <col min="6" max="6" width="11.575" style="26" customWidth="1"/>
+    <col min="7" max="7" width="11.1416666666667" customWidth="1"/>
     <col min="8" max="8" width="10" style="26" customWidth="1"/>
-    <col min="9" max="9" width="13.5714285714286" style="26" customWidth="1"/>
-    <col min="10" max="10" width="13.5714285714286" customWidth="1"/>
-    <col min="11" max="11" width="11.7142857142857" style="26"/>
-    <col min="12" max="14" width="10.5714285714286" customWidth="1"/>
+    <col min="9" max="9" width="13.575" style="26" customWidth="1"/>
+    <col min="10" max="10" width="13.575" customWidth="1"/>
+    <col min="11" max="11" width="11.7166666666667" style="26"/>
+    <col min="12" max="14" width="10.575" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -7115,7 +7138,7 @@
       </c>
     </row>
     <row r="130" spans="1:11">
-      <c r="A130" s="55" t="s">
+      <c r="A130" s="56" t="s">
         <v>239</v>
       </c>
       <c r="B130" s="33">
@@ -7152,7 +7175,7 @@
       </c>
     </row>
     <row r="131" spans="1:11">
-      <c r="A131" s="55" t="s">
+      <c r="A131" s="56" t="s">
         <v>241</v>
       </c>
       <c r="B131" s="33">
@@ -7187,7 +7210,7 @@
       </c>
     </row>
     <row r="132" spans="1:11">
-      <c r="A132" s="55" t="s">
+      <c r="A132" s="56" t="s">
         <v>244</v>
       </c>
       <c r="B132" s="33">
@@ -7224,7 +7247,7 @@
       </c>
     </row>
     <row r="133" spans="1:11">
-      <c r="A133" s="55" t="s">
+      <c r="A133" s="56" t="s">
         <v>246</v>
       </c>
       <c r="B133" s="33">
@@ -7298,7 +7321,7 @@
       </c>
     </row>
     <row r="135" spans="1:11">
-      <c r="A135" s="55" t="s">
+      <c r="A135" s="56" t="s">
         <v>252</v>
       </c>
       <c r="B135" s="33">
@@ -7335,7 +7358,7 @@
       </c>
     </row>
     <row r="136" spans="1:11">
-      <c r="A136" s="55" t="s">
+      <c r="A136" s="56" t="s">
         <v>253</v>
       </c>
       <c r="B136" s="33">
@@ -7372,7 +7395,7 @@
       </c>
     </row>
     <row r="137" spans="1:11">
-      <c r="A137" s="55" t="s">
+      <c r="A137" s="56" t="s">
         <v>256</v>
       </c>
       <c r="B137" s="33">
@@ -7409,7 +7432,7 @@
       </c>
     </row>
     <row r="138" spans="1:11">
-      <c r="A138" s="55" t="s">
+      <c r="A138" s="56" t="s">
         <v>258</v>
       </c>
       <c r="B138" s="33">
@@ -7443,7 +7466,7 @@
       </c>
     </row>
     <row r="139" spans="1:11">
-      <c r="A139" s="55" t="s">
+      <c r="A139" s="56" t="s">
         <v>259</v>
       </c>
       <c r="B139" s="33">
@@ -7702,7 +7725,7 @@
       </c>
     </row>
     <row r="146" spans="1:11">
-      <c r="A146" s="55" t="s">
+      <c r="A146" s="56" t="s">
         <v>270</v>
       </c>
       <c r="B146" s="33">
@@ -7736,7 +7759,7 @@
       </c>
     </row>
     <row r="147" spans="1:11">
-      <c r="A147" s="55" t="s">
+      <c r="A147" s="56" t="s">
         <v>273</v>
       </c>
       <c r="B147" s="33">
@@ -7770,7 +7793,7 @@
       </c>
     </row>
     <row r="148" spans="1:11">
-      <c r="A148" s="55" t="s">
+      <c r="A148" s="56" t="s">
         <v>275</v>
       </c>
       <c r="B148" s="33">
@@ -7804,7 +7827,7 @@
       </c>
     </row>
     <row r="149" spans="1:11">
-      <c r="A149" s="55" t="s">
+      <c r="A149" s="56" t="s">
         <v>277</v>
       </c>
       <c r="B149" s="33">
@@ -7838,7 +7861,7 @@
       </c>
     </row>
     <row r="150" spans="1:11">
-      <c r="A150" s="55" t="s">
+      <c r="A150" s="56" t="s">
         <v>279</v>
       </c>
       <c r="B150" s="33">
@@ -7869,7 +7892,7 @@
       </c>
     </row>
     <row r="151" spans="1:11">
-      <c r="A151" s="55" t="s">
+      <c r="A151" s="56" t="s">
         <v>280</v>
       </c>
       <c r="B151" s="33">
@@ -7940,7 +7963,7 @@
       </c>
     </row>
     <row r="153" spans="1:11">
-      <c r="A153" s="55" t="s">
+      <c r="A153" s="56" t="s">
         <v>286</v>
       </c>
       <c r="B153" s="33">
@@ -7974,7 +7997,7 @@
       </c>
     </row>
     <row r="154" spans="1:11">
-      <c r="A154" s="55" t="s">
+      <c r="A154" s="56" t="s">
         <v>287</v>
       </c>
       <c r="B154" s="33">
@@ -8045,7 +8068,7 @@
       </c>
     </row>
     <row r="156" spans="1:11">
-      <c r="A156" s="55" t="s">
+      <c r="A156" s="56" t="s">
         <v>292</v>
       </c>
       <c r="B156" s="33">
@@ -8116,7 +8139,7 @@
       </c>
     </row>
     <row r="158" spans="1:11">
-      <c r="A158" s="55" t="s">
+      <c r="A158" s="56" t="s">
         <v>295</v>
       </c>
       <c r="B158" s="33">
@@ -8187,7 +8210,7 @@
       </c>
     </row>
     <row r="160" spans="1:11">
-      <c r="A160" s="55" t="s">
+      <c r="A160" s="56" t="s">
         <v>297</v>
       </c>
       <c r="B160" s="33">
@@ -8258,7 +8281,7 @@
       </c>
     </row>
     <row r="162" spans="1:11">
-      <c r="A162" s="55" t="s">
+      <c r="A162" s="56" t="s">
         <v>301</v>
       </c>
       <c r="B162" s="33">
@@ -8292,7 +8315,7 @@
       </c>
     </row>
     <row r="163" spans="1:11">
-      <c r="A163" s="55" t="s">
+      <c r="A163" s="56" t="s">
         <v>302</v>
       </c>
       <c r="B163" s="33">
@@ -8326,7 +8349,7 @@
       </c>
     </row>
     <row r="164" spans="1:11">
-      <c r="A164" s="55" t="s">
+      <c r="A164" s="56" t="s">
         <v>303</v>
       </c>
       <c r="B164" s="33">
@@ -8357,7 +8380,7 @@
       </c>
     </row>
     <row r="165" spans="1:11">
-      <c r="A165" s="55" t="s">
+      <c r="A165" s="56" t="s">
         <v>306</v>
       </c>
       <c r="B165" s="33">
@@ -8391,7 +8414,7 @@
       </c>
     </row>
     <row r="166" spans="1:11">
-      <c r="A166" s="55" t="s">
+      <c r="A166" s="56" t="s">
         <v>307</v>
       </c>
       <c r="B166" s="33">
@@ -8425,7 +8448,7 @@
       </c>
     </row>
     <row r="167" spans="1:11">
-      <c r="A167" s="55" t="s">
+      <c r="A167" s="56" t="s">
         <v>310</v>
       </c>
       <c r="B167" s="33">
@@ -8589,7 +8612,7 @@
       </c>
     </row>
     <row r="172" spans="1:11">
-      <c r="A172" s="55" t="s">
+      <c r="A172" s="56" t="s">
         <v>318</v>
       </c>
       <c r="B172" s="33">
@@ -9641,7 +9664,7 @@
       <c r="C201" t="s">
         <v>97</v>
       </c>
-      <c r="D201" s="56" t="s">
+      <c r="D201" s="57" t="s">
         <v>361</v>
       </c>
       <c r="F201" s="26">
@@ -10425,7 +10448,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="224" ht="30" spans="1:11">
+    <row r="224" spans="1:11">
       <c r="A224" s="23" t="s">
         <v>398</v>
       </c>
@@ -11041,7 +11064,7 @@
       <c r="C242" t="s">
         <v>438</v>
       </c>
-      <c r="D242" s="56" t="s">
+      <c r="D242" s="57" t="s">
         <v>361</v>
       </c>
       <c r="F242" s="26">
@@ -11810,7 +11833,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="265" ht="30" spans="1:11">
+    <row r="265" spans="1:11">
       <c r="A265" s="49" t="s">
         <v>468</v>
       </c>
@@ -12622,7 +12645,7 @@
         <v>100000</v>
       </c>
       <c r="G289" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H289" s="26">
         <v>98500</v>
@@ -12640,7 +12663,7 @@
       </c>
     </row>
     <row r="290" spans="1:11">
-      <c r="A290" s="53" t="s">
+      <c r="A290" s="49" t="s">
         <v>505</v>
       </c>
       <c r="B290" s="33">
@@ -12677,7 +12700,7 @@
       </c>
     </row>
     <row r="291" spans="1:11">
-      <c r="A291" s="53" t="s">
+      <c r="A291" s="49" t="s">
         <v>494</v>
       </c>
       <c r="B291" s="33">
@@ -12714,7 +12737,7 @@
       </c>
     </row>
     <row r="292" spans="1:11">
-      <c r="A292" s="53" t="s">
+      <c r="A292" s="49" t="s">
         <v>495</v>
       </c>
       <c r="B292" s="33">
@@ -12745,7 +12768,7 @@
       </c>
     </row>
     <row r="293" ht="15.75" spans="1:11">
-      <c r="A293" s="53" t="s">
+      <c r="A293" s="49" t="s">
         <v>496</v>
       </c>
       <c r="B293" s="33">
@@ -12779,7 +12802,7 @@
       </c>
     </row>
     <row r="294" spans="1:11">
-      <c r="A294" s="53" t="s">
+      <c r="A294" s="49" t="s">
         <v>497</v>
       </c>
       <c r="B294" s="33">
@@ -12813,7 +12836,7 @@
       </c>
     </row>
     <row r="295" spans="1:11">
-      <c r="A295" s="53" t="s">
+      <c r="A295" s="49" t="s">
         <v>501</v>
       </c>
       <c r="B295" s="33">
@@ -12843,126 +12866,309 @@
         <v>775</v>
       </c>
     </row>
-    <row r="296" spans="2:11">
+    <row r="296" spans="1:11">
+      <c r="A296" s="53" t="s">
+        <v>502</v>
+      </c>
       <c r="B296" s="33">
         <v>42886</v>
       </c>
+      <c r="C296" t="s">
+        <v>142</v>
+      </c>
+      <c r="D296" s="58" t="s">
+        <v>143</v>
+      </c>
+      <c r="E296" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="F296" s="26">
+        <v>21500</v>
+      </c>
+      <c r="G296" t="s">
+        <v>16</v>
+      </c>
+      <c r="H296" s="26">
+        <v>21500</v>
+      </c>
       <c r="J296" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1075</v>
       </c>
       <c r="K296" s="26">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="297" spans="2:11">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="297" spans="1:11">
+      <c r="A297" s="53" t="s">
+        <v>503</v>
+      </c>
       <c r="B297" s="33">
         <v>42886</v>
       </c>
+      <c r="C297" t="s">
+        <v>355</v>
+      </c>
+      <c r="D297" s="24" t="s">
+        <v>504</v>
+      </c>
+      <c r="F297" s="26">
+        <v>100000</v>
+      </c>
+      <c r="G297" t="s">
+        <v>12</v>
+      </c>
+      <c r="H297" s="26">
+        <v>98500</v>
+      </c>
       <c r="J297" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4925</v>
       </c>
       <c r="K297" s="26">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="298" spans="2:11">
+        <v>6425</v>
+      </c>
+    </row>
+    <row r="298" spans="1:11">
+      <c r="A298" s="53" t="s">
+        <v>508</v>
+      </c>
       <c r="B298" s="33">
-        <v>42886</v>
+        <v>42887</v>
+      </c>
+      <c r="C298" t="s">
+        <v>142</v>
+      </c>
+      <c r="D298" s="24" t="s">
+        <v>509</v>
+      </c>
+      <c r="E298" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="F298" s="26">
+        <v>11300</v>
+      </c>
+      <c r="G298" t="s">
+        <v>12</v>
+      </c>
+      <c r="H298" s="26">
+        <v>11300</v>
       </c>
       <c r="J298" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>565</v>
       </c>
       <c r="K298" s="26">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="299" spans="2:11">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="299" spans="1:11">
+      <c r="A299" s="53" t="s">
+        <v>510</v>
+      </c>
       <c r="B299" s="33">
-        <v>42886</v>
+        <v>42887</v>
+      </c>
+      <c r="C299" t="s">
+        <v>90</v>
+      </c>
+      <c r="D299" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="E299" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F299" s="26">
+        <v>50000</v>
+      </c>
+      <c r="G299" t="s">
+        <v>16</v>
+      </c>
+      <c r="H299" s="26">
+        <v>51500</v>
       </c>
       <c r="J299" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>2575</v>
       </c>
       <c r="K299" s="26">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="300" spans="2:11">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="300" spans="1:11">
+      <c r="A300" s="53" t="s">
+        <v>511</v>
+      </c>
       <c r="B300" s="33">
-        <v>42886</v>
+        <v>42887</v>
+      </c>
+      <c r="C300" t="s">
+        <v>438</v>
+      </c>
+      <c r="D300" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="E300" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F300" s="26">
+        <v>200000</v>
+      </c>
+      <c r="G300" t="s">
+        <v>16</v>
+      </c>
+      <c r="H300" s="26">
+        <v>201500</v>
       </c>
       <c r="J300" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>10075</v>
       </c>
       <c r="K300" s="26">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="301" spans="2:11">
+        <v>8575</v>
+      </c>
+    </row>
+    <row r="301" spans="1:11">
+      <c r="A301" s="53" t="s">
+        <v>512</v>
+      </c>
       <c r="B301" s="33">
-        <v>42886</v>
+        <v>42887</v>
+      </c>
+      <c r="C301" t="s">
+        <v>438</v>
+      </c>
+      <c r="D301" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="F301" s="26">
+        <v>50000</v>
+      </c>
+      <c r="G301" t="s">
+        <v>12</v>
+      </c>
+      <c r="H301" s="26">
+        <v>49000</v>
       </c>
       <c r="J301" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="K301" s="26">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="302" spans="2:11">
+        <v>3450</v>
+      </c>
+    </row>
+    <row r="302" spans="1:11">
+      <c r="A302" s="53" t="s">
+        <v>513</v>
+      </c>
       <c r="B302" s="33">
-        <v>42886</v>
+        <v>42887</v>
+      </c>
+      <c r="C302" t="s">
+        <v>78</v>
+      </c>
+      <c r="D302" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E302" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F302" s="26">
+        <v>21000</v>
+      </c>
+      <c r="G302" t="s">
+        <v>16</v>
+      </c>
+      <c r="H302" s="26">
+        <v>20500</v>
       </c>
       <c r="J302" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1025</v>
       </c>
       <c r="K302" s="26">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="303" spans="2:11">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="303" spans="1:11">
+      <c r="A303" s="53" t="s">
+        <v>514</v>
+      </c>
       <c r="B303" s="33">
-        <v>42886</v>
+        <v>42887</v>
+      </c>
+      <c r="C303" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D303" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="E303" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="F303" s="34">
+        <v>25500</v>
+      </c>
+      <c r="G303" t="s">
+        <v>12</v>
+      </c>
+      <c r="H303" s="26">
+        <v>24800</v>
       </c>
       <c r="J303" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1240</v>
       </c>
       <c r="K303" s="26">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="304" spans="2:11">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="304" spans="1:11">
+      <c r="A304" s="55" t="s">
+        <v>515</v>
+      </c>
       <c r="B304" s="33">
-        <v>42886</v>
+        <v>42887</v>
+      </c>
+      <c r="C304" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D304" s="24" t="s">
+        <v>516</v>
+      </c>
+      <c r="E304" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="F304" s="26">
+        <v>12000</v>
+      </c>
+      <c r="G304" t="s">
+        <v>12</v>
+      </c>
+      <c r="H304" s="26">
+        <v>11300</v>
       </c>
       <c r="J304" s="38">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>565</v>
       </c>
       <c r="K304" s="26">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="305" spans="2:11">
       <c r="B305" s="33">
-        <v>42886</v>
+        <v>42887</v>
       </c>
       <c r="J305" s="38">
         <f t="shared" si="10"/>
@@ -12975,7 +13181,7 @@
     </row>
     <row r="306" spans="2:11">
       <c r="B306" s="33">
-        <v>42886</v>
+        <v>42887</v>
       </c>
       <c r="J306" s="38">
         <f t="shared" si="10"/>
@@ -12988,7 +13194,7 @@
     </row>
     <row r="307" spans="2:11">
       <c r="B307" s="33">
-        <v>42886</v>
+        <v>42887</v>
       </c>
       <c r="J307" s="38">
         <f t="shared" si="10"/>
@@ -13001,7 +13207,7 @@
     </row>
     <row r="308" spans="2:11">
       <c r="B308" s="33">
-        <v>42886</v>
+        <v>42887</v>
       </c>
       <c r="J308" s="38">
         <f t="shared" si="10"/>
@@ -13728,6 +13934,15 @@
     <hyperlink ref="A293" r:id="rId103" display="BL17113DGJA3INV" tooltip="https://www.bukalapak.com/payment/invoices/123716742"/>
     <hyperlink ref="A294" r:id="rId104" display="BL171111UJXSELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1266572"/>
     <hyperlink ref="A295" r:id="rId105" display="BL17113DIZLNINV" tooltip="https://www.bukalapak.com/payment/invoices/123822497"/>
+    <hyperlink ref="A296" r:id="rId106" display="BL171111UK63ELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1266827"/>
+    <hyperlink ref="A297" r:id="rId107" display="BL17113DKEL3INV" tooltip="https://www.bukalapak.com/payment/invoices/123882502"/>
+    <hyperlink ref="A298" r:id="rId109" display="BL17113DSL3NINV" tooltip="https://www.bukalapak.com/payment/invoices/124233467"/>
+    <hyperlink ref="A299" r:id="rId110" display="BL171111VECXELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1302592"/>
+    <hyperlink ref="A300" r:id="rId111" display="BL171111VPTXELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1316662"/>
+    <hyperlink ref="A301" r:id="rId112" display="BL17113EBDX8INV" tooltip="https://www.bukalapak.com/payment/invoices/124996452"/>
+    <hyperlink ref="A302" r:id="rId113" display="BL171111W3C8ELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/1331967"/>
+    <hyperlink ref="A303" r:id="rId114" display="BL17113EH6LNINV" tooltip="https://www.bukalapak.com/payment/invoices/125244722"/>
+    <hyperlink ref="A304" r:id="rId115" display="BL17113EH7J8INV" tooltip="https://www.bukalapak.com/payment/invoices/125245862"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -13746,28 +13961,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="24.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="13.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="20.2857142857143" customWidth="1"/>
-    <col min="4" max="4" width="26.7142857142857" customWidth="1"/>
-    <col min="5" max="5" width="13.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="24.1416666666667" customWidth="1"/>
+    <col min="2" max="2" width="13.8583333333333" customWidth="1"/>
+    <col min="3" max="3" width="20.2833333333333" customWidth="1"/>
+    <col min="4" max="4" width="26.7166666666667" customWidth="1"/>
+    <col min="5" max="5" width="13.7166666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="20" t="s">
-        <v>508</v>
+        <v>517</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>509</v>
+        <v>518</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>510</v>
+        <v>519</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>511</v>
+        <v>520</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>512</v>
+        <v>521</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -14044,7 +14259,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
-        <v>513</v>
+        <v>522</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -14056,7 +14271,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="21" t="s">
-        <v>514</v>
+        <v>523</v>
       </c>
       <c r="E20" s="22">
         <f>5%*E18</f>
@@ -14065,7 +14280,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="21" t="s">
-        <v>515</v>
+        <v>524</v>
       </c>
       <c r="E21" s="22">
         <f>10%*E18</f>
@@ -14092,32 +14307,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="11.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="15.2857142857143" customWidth="1"/>
+    <col min="1" max="1" width="11.575" customWidth="1"/>
+    <col min="2" max="2" width="15.2833333333333" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="20.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="20.2833333333333" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="14.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="14.1416666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>516</v>
+        <v>525</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>517</v>
+        <v>526</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>518</v>
+        <v>527</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>519</v>
+        <v>528</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -14196,7 +14411,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="7" t="s">
-        <v>520</v>
+        <v>529</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -14209,7 +14424,7 @@
     </row>
     <row r="9" spans="4:5">
       <c r="D9" s="11" t="s">
-        <v>521</v>
+        <v>530</v>
       </c>
       <c r="E9" s="12">
         <v>1000000</v>
@@ -14217,7 +14432,7 @@
     </row>
     <row r="10" spans="4:5">
       <c r="D10" s="13" t="s">
-        <v>522</v>
+        <v>531</v>
       </c>
       <c r="E10" s="5">
         <f>E9-E6</f>
@@ -14230,7 +14445,7 @@
     </row>
     <row r="12" spans="4:5">
       <c r="D12" s="3" t="s">
-        <v>523</v>
+        <v>532</v>
       </c>
       <c r="E12" s="5">
         <v>300000</v>
@@ -14238,7 +14453,7 @@
     </row>
     <row r="13" spans="4:5">
       <c r="D13" s="13" t="s">
-        <v>524</v>
+        <v>533</v>
       </c>
       <c r="E13" s="5">
         <v>300000</v>
@@ -14246,7 +14461,7 @@
     </row>
     <row r="14" spans="4:5">
       <c r="D14" s="11" t="s">
-        <v>525</v>
+        <v>534</v>
       </c>
       <c r="E14" s="12">
         <f>E13+E12</f>
@@ -14259,7 +14474,7 @@
     </row>
     <row r="16" spans="4:5">
       <c r="D16" s="11" t="s">
-        <v>526</v>
+        <v>535</v>
       </c>
       <c r="E16" s="12">
         <f>E10-E14</f>
@@ -14494,7 +14709,7 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="16" t="s">
-        <v>520</v>
+        <v>529</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -14507,7 +14722,7 @@
     </row>
     <row r="34" spans="4:5">
       <c r="D34" s="11" t="s">
-        <v>527</v>
+        <v>536</v>
       </c>
       <c r="E34" s="19">
         <f>E16</f>
@@ -14524,7 +14739,7 @@
     </row>
     <row r="36" spans="4:5">
       <c r="D36" s="11" t="s">
-        <v>528</v>
+        <v>537</v>
       </c>
       <c r="E36" s="19">
         <f>E34+E35</f>
@@ -14537,7 +14752,7 @@
     </row>
     <row r="38" spans="4:5">
       <c r="D38" s="11" t="s">
-        <v>529</v>
+        <v>538</v>
       </c>
       <c r="E38" s="19">
         <f>E36-E32</f>

</xml_diff>

<commit_message>
tgl 26 blm sls
</commit_message>
<xml_diff>
--- a/Jual Pulsa.xlsx
+++ b/Jual Pulsa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23400" windowHeight="11385" activeTab="1"/>
+    <workbookView windowWidth="20385" windowHeight="8370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet5" sheetId="5" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Ustadz Fauzan" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$B$1:$I$626</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$B$1:$I$633</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <pivotCaches>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984">
   <si>
     <t>Dibayar</t>
   </si>
@@ -2877,6 +2877,27 @@
   </si>
   <si>
     <t>BL171114TI8MELC </t>
+  </si>
+  <si>
+    <t>BL171114TRVXELC </t>
+  </si>
+  <si>
+    <t>BL171114U1Y8ELC</t>
+  </si>
+  <si>
+    <t>BL17114EY4AIINV</t>
+  </si>
+  <si>
+    <t>BL171114USZXELC </t>
+  </si>
+  <si>
+    <t>BL171114UTB8ELC </t>
+  </si>
+  <si>
+    <t>BL17114EYMOXINV</t>
+  </si>
+  <si>
+    <t>BL171114UTISELC</t>
   </si>
   <si>
     <t>NO TRANSAKSI</t>
@@ -2962,12 +2983,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="28">
@@ -3032,14 +3053,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -3047,19 +3060,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3072,14 +3076,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3102,22 +3138,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -3132,16 +3153,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3156,21 +3184,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3203,13 +3224,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3221,19 +3248,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3251,37 +3326,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3293,25 +3356,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3323,67 +3392,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3569,6 +3590,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3586,24 +3631,20 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3619,17 +3660,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3657,23 +3687,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3685,160 +3706,160 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3860,7 +3881,7 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -3891,12 +3912,12 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3931,26 +3952,25 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
@@ -4007,16 +4027,16 @@
   </cellStyles>
   <dxfs count="154">
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="180" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??.0_);_(@_)"/>
@@ -4037,412 +4057,412 @@
       <numFmt numFmtId="183" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy;@"/>
+      <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="184" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??.0_);_(@_)"/>
@@ -4463,10 +4483,10 @@
       <numFmt numFmtId="187" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -4509,7 +4529,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="105410" y="2638425"/>
-          <a:ext cx="3641090" cy="2838450"/>
+          <a:ext cx="3314700" cy="2838450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5597,7 +5617,7 @@
         <s v="M. SYARIFUDDIN"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Harga" numFmtId="177">
+    <cacheField name="Harga" numFmtId="176">
       <sharedItems containsBlank="1" containsNumber="1" containsInteger="1" containsMixedTypes="1" count="52">
         <m/>
         <s v="Deposit"/>
@@ -5664,7 +5684,7 @@
         <s v="Listrik Pasca"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Nominal" numFmtId="177">
+    <cacheField name="Nominal" numFmtId="176">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="5000" maxValue="510000" count="61">
         <n v="57000"/>
         <n v="11000"/>
@@ -5729,7 +5749,7 @@
         <n v="78500"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Dibayar" numFmtId="177">
+    <cacheField name="Dibayar" numFmtId="176">
       <sharedItems containsBlank="1" containsNumber="1" containsInteger="1" containsMixedTypes="1" count="60">
         <n v="57000"/>
         <n v="12000"/>
@@ -5859,7 +5879,7 @@
         <m/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Laba" numFmtId="177">
+    <cacheField name="Laba" numFmtId="176">
       <sharedItems containsBlank="1" containsNumber="1" containsMixedTypes="1" count="103">
         <n v="-54150"/>
         <n v="-10450"/>
@@ -17091,288 +17111,288 @@
       </pivotSelection>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="21.425" customWidth="1"/>
-    <col min="2" max="2" width="15.1416666666667" style="15" customWidth="1"/>
-    <col min="3" max="3" width="27.8083333333333" customWidth="1"/>
-    <col min="4" max="4" width="20.8583333333333" customWidth="1"/>
-    <col min="5" max="5" width="25.425" customWidth="1"/>
-    <col min="6" max="6" width="13.8583333333333"/>
-    <col min="7" max="7" width="14.425" style="18"/>
+    <col min="1" max="1" width="21.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="15.1428571428571" style="15" customWidth="1"/>
+    <col min="3" max="3" width="27.8095238095238" customWidth="1"/>
+    <col min="4" max="4" width="20.8571428571429" customWidth="1"/>
+    <col min="5" max="5" width="25.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="13.8571428571429"/>
+    <col min="7" max="7" width="14.4285714285714" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="75" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="77" t="s">
+      <c r="E3" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="77" t="s">
+      <c r="F3" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="79" t="s">
+      <c r="G3" s="78" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="80">
+      <c r="B4" s="79">
         <v>42862</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="81" t="s">
+      <c r="E4" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="81" t="s">
+      <c r="F4" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="79">
+      <c r="G4" s="78">
         <v>50000</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="83">
+      <c r="B5" s="82">
         <v>42883</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="84" t="s">
+      <c r="E5" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="84" t="s">
+      <c r="F5" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="85">
+      <c r="G5" s="84">
         <v>200000</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="83">
+      <c r="B6" s="82">
         <v>42920</v>
       </c>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="84" t="s">
+      <c r="D6" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="84" t="s">
+      <c r="E6" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="84" t="s">
+      <c r="F6" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="85">
+      <c r="G6" s="84">
         <v>100000</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="83">
+      <c r="B7" s="82">
         <v>42946</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="84" t="s">
+      <c r="E7" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="84" t="s">
+      <c r="F7" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="85">
+      <c r="G7" s="84">
         <v>100000</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="83">
+      <c r="B8" s="82">
         <v>42946</v>
       </c>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="84" t="s">
+      <c r="D8" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="84" t="s">
+      <c r="E8" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="84" t="s">
+      <c r="F8" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="85">
+      <c r="G8" s="84">
         <v>100000</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="82" t="s">
+      <c r="A9" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="83">
+      <c r="B9" s="82">
         <v>42962</v>
       </c>
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="84" t="s">
+      <c r="D9" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="84" t="s">
+      <c r="E9" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="84" t="s">
+      <c r="F9" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="85">
+      <c r="G9" s="84">
         <v>100000</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="83">
+      <c r="B10" s="82">
         <v>42869</v>
       </c>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="84" t="s">
+      <c r="D10" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="84" t="s">
+      <c r="E10" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="84" t="s">
+      <c r="F10" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="85">
+      <c r="G10" s="84">
         <v>50500</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="82" t="s">
+      <c r="A11" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="83">
+      <c r="B11" s="82">
         <v>42882</v>
       </c>
-      <c r="C11" s="84" t="s">
+      <c r="C11" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="84" t="s">
+      <c r="E11" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="84" t="s">
+      <c r="F11" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="85">
+      <c r="G11" s="84">
         <v>50000</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="82" t="s">
+      <c r="A12" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="83">
+      <c r="B12" s="82">
         <v>42883</v>
       </c>
-      <c r="C12" s="84" t="s">
+      <c r="C12" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="84" t="s">
+      <c r="D12" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="84" t="s">
+      <c r="E12" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="84" t="s">
+      <c r="F12" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="85">
+      <c r="G12" s="84">
         <v>50500</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="83">
+      <c r="B13" s="82">
         <v>42938</v>
       </c>
-      <c r="C13" s="84" t="s">
+      <c r="C13" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D13" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="84" t="s">
+      <c r="E13" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="84" t="s">
+      <c r="F13" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="85">
+      <c r="G13" s="84">
         <v>50000</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="86" t="s">
+      <c r="A14" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="87"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="89">
+      <c r="B14" s="86"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="88">
         <v>851000</v>
       </c>
     </row>
@@ -17751,27 +17771,27 @@
   <dimension ref="A1:N643"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B610" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B627" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B633" sqref="B633:G633"/>
+      <selection pane="bottomRight" activeCell="H640" sqref="H640"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.7166666666667" style="14" customWidth="1"/>
-    <col min="2" max="2" width="9.71666666666667" customWidth="1"/>
-    <col min="3" max="3" width="21.375" customWidth="1"/>
-    <col min="4" max="4" width="25.2833333333333" style="16" customWidth="1"/>
-    <col min="5" max="5" width="11.875" style="41" customWidth="1"/>
-    <col min="6" max="6" width="11.575" style="18" customWidth="1"/>
-    <col min="7" max="7" width="11.1416666666667" customWidth="1"/>
+    <col min="1" max="1" width="22.7142857142857" style="14" customWidth="1"/>
+    <col min="2" max="2" width="9.71428571428571" customWidth="1"/>
+    <col min="3" max="3" width="21.3714285714286" customWidth="1"/>
+    <col min="4" max="4" width="25.2857142857143" style="16" customWidth="1"/>
+    <col min="5" max="5" width="11.8761904761905" style="41" customWidth="1"/>
+    <col min="6" max="6" width="11.5714285714286" style="18" customWidth="1"/>
+    <col min="7" max="7" width="11.1428571428571" customWidth="1"/>
     <col min="8" max="8" width="10" style="18" customWidth="1"/>
-    <col min="9" max="9" width="13.575" style="18" customWidth="1"/>
-    <col min="10" max="10" width="13.575" customWidth="1"/>
-    <col min="11" max="11" width="11.7166666666667" style="18"/>
-    <col min="12" max="14" width="10.575" customWidth="1"/>
+    <col min="9" max="9" width="13.5714285714286" style="18" customWidth="1"/>
+    <col min="10" max="10" width="13.5714285714286" customWidth="1"/>
+    <col min="11" max="11" width="11.7142857142857" style="18"/>
+    <col min="12" max="14" width="10.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -17933,7 +17953,7 @@
         <v>-48925</v>
       </c>
     </row>
-    <row r="7" ht="30" spans="1:11">
+    <row r="7" ht="45" spans="1:11">
       <c r="A7" s="16"/>
       <c r="B7" s="48">
         <v>42825</v>
@@ -18401,7 +18421,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" ht="30" spans="1:11">
+    <row r="23" ht="45" spans="1:11">
       <c r="A23" s="16"/>
       <c r="B23" s="48">
         <v>42833</v>
@@ -18582,7 +18602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" ht="30" spans="1:12">
       <c r="A29" s="16"/>
       <c r="B29" s="48">
         <v>42834</v>
@@ -19082,7 +19102,7 @@
       </c>
       <c r="L43" s="52"/>
     </row>
-    <row r="44" ht="30" spans="1:12">
+    <row r="44" ht="45" spans="1:12">
       <c r="A44" s="16"/>
       <c r="B44" s="48">
         <v>42840</v>
@@ -19118,7 +19138,7 @@
       </c>
       <c r="L44" s="52"/>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" ht="30" spans="1:11">
       <c r="A45" s="16"/>
       <c r="B45" s="48">
         <v>42840</v>
@@ -19319,7 +19339,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" ht="30" spans="1:11">
       <c r="A51" s="16"/>
       <c r="B51" s="48">
         <v>42841</v>
@@ -19418,7 +19438,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="54" ht="30" spans="1:11">
+    <row r="54" ht="45" spans="1:11">
       <c r="A54" s="16"/>
       <c r="B54" s="48">
         <v>42841</v>
@@ -19657,7 +19677,7 @@
         <v>21075</v>
       </c>
     </row>
-    <row r="61" ht="30" spans="1:11">
+    <row r="61" ht="45" spans="1:11">
       <c r="A61" s="16"/>
       <c r="B61" s="48">
         <v>42843</v>
@@ -20104,7 +20124,7 @@
         <v>2575</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" ht="30" spans="1:11">
       <c r="A74" s="16"/>
       <c r="B74" s="48">
         <v>42845</v>
@@ -20244,7 +20264,7 @@
         <v>2575</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" ht="30" spans="1:11">
       <c r="A78" s="16" t="s">
         <v>162</v>
       </c>
@@ -20352,7 +20372,7 @@
         <v>8575</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" ht="30" spans="1:11">
       <c r="A81" s="16" t="s">
         <v>169</v>
       </c>
@@ -20463,7 +20483,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="84" ht="30" spans="1:11">
+    <row r="84" ht="45" spans="1:11">
       <c r="A84" s="16" t="s">
         <v>178</v>
       </c>
@@ -20784,7 +20804,7 @@
       <c r="M92" s="52"/>
       <c r="N92" s="52"/>
     </row>
-    <row r="93" ht="30" spans="1:11">
+    <row r="93" ht="45" spans="1:11">
       <c r="A93" s="54" t="s">
         <v>197</v>
       </c>
@@ -21763,7 +21783,7 @@
         <v>8575</v>
       </c>
     </row>
-    <row r="121" spans="1:11">
+    <row r="121" ht="30" spans="1:11">
       <c r="A121" s="16"/>
       <c r="B121" s="48">
         <v>42855</v>
@@ -21937,7 +21957,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="126" spans="1:11">
+    <row r="126" ht="30" spans="1:11">
       <c r="A126" s="57" t="s">
         <v>253</v>
       </c>
@@ -22082,8 +22102,8 @@
         <v>18575</v>
       </c>
     </row>
-    <row r="130" spans="1:11">
-      <c r="A130" s="90" t="s">
+    <row r="130" ht="30" spans="1:11">
+      <c r="A130" s="89" t="s">
         <v>259</v>
       </c>
       <c r="B130" s="48">
@@ -22120,7 +22140,7 @@
       </c>
     </row>
     <row r="131" ht="30" spans="1:11">
-      <c r="A131" s="90" t="s">
+      <c r="A131" s="89" t="s">
         <v>261</v>
       </c>
       <c r="B131" s="48">
@@ -22154,8 +22174,8 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="132" spans="1:11">
-      <c r="A132" s="90" t="s">
+    <row r="132" ht="30" spans="1:11">
+      <c r="A132" s="89" t="s">
         <v>264</v>
       </c>
       <c r="B132" s="48">
@@ -22191,8 +22211,8 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="133" spans="1:11">
-      <c r="A133" s="90" t="s">
+    <row r="133" ht="30" spans="1:11">
+      <c r="A133" s="89" t="s">
         <v>266</v>
       </c>
       <c r="B133" s="48">
@@ -22266,7 +22286,7 @@
       </c>
     </row>
     <row r="135" spans="1:11">
-      <c r="A135" s="90" t="s">
+      <c r="A135" s="89" t="s">
         <v>272</v>
       </c>
       <c r="B135" s="48">
@@ -22302,8 +22322,8 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="136" spans="1:11">
-      <c r="A136" s="90" t="s">
+    <row r="136" ht="30" spans="1:11">
+      <c r="A136" s="89" t="s">
         <v>273</v>
       </c>
       <c r="B136" s="48">
@@ -22339,8 +22359,8 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="137" spans="1:11">
-      <c r="A137" s="90" t="s">
+    <row r="137" ht="30" spans="1:11">
+      <c r="A137" s="89" t="s">
         <v>276</v>
       </c>
       <c r="B137" s="48">
@@ -22377,7 +22397,7 @@
       </c>
     </row>
     <row r="138" spans="1:11">
-      <c r="A138" s="90" t="s">
+      <c r="A138" s="89" t="s">
         <v>278</v>
       </c>
       <c r="B138" s="48">
@@ -22411,7 +22431,7 @@
       </c>
     </row>
     <row r="139" spans="1:11">
-      <c r="A139" s="90" t="s">
+      <c r="A139" s="89" t="s">
         <v>279</v>
       </c>
       <c r="B139" s="48">
@@ -22484,7 +22504,7 @@
         <v>8575</v>
       </c>
     </row>
-    <row r="141" spans="1:11">
+    <row r="141" ht="30" spans="1:11">
       <c r="A141" s="14" t="s">
         <v>281</v>
       </c>
@@ -22521,7 +22541,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="142" ht="30" spans="1:11">
+    <row r="142" ht="45" spans="1:11">
       <c r="A142" s="14" t="s">
         <v>282</v>
       </c>
@@ -22558,7 +22578,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="143" spans="1:11">
+    <row r="143" ht="30" spans="1:11">
       <c r="A143" s="14" t="s">
         <v>285</v>
       </c>
@@ -22670,7 +22690,7 @@
       </c>
     </row>
     <row r="146" spans="1:11">
-      <c r="A146" s="90" t="s">
+      <c r="A146" s="89" t="s">
         <v>289</v>
       </c>
       <c r="B146" s="48">
@@ -22704,7 +22724,7 @@
       </c>
     </row>
     <row r="147" spans="1:11">
-      <c r="A147" s="90" t="s">
+      <c r="A147" s="89" t="s">
         <v>292</v>
       </c>
       <c r="B147" s="48">
@@ -22738,7 +22758,7 @@
       </c>
     </row>
     <row r="148" spans="1:11">
-      <c r="A148" s="90" t="s">
+      <c r="A148" s="89" t="s">
         <v>294</v>
       </c>
       <c r="B148" s="48">
@@ -22772,7 +22792,7 @@
       </c>
     </row>
     <row r="149" spans="1:11">
-      <c r="A149" s="90" t="s">
+      <c r="A149" s="89" t="s">
         <v>296</v>
       </c>
       <c r="B149" s="48">
@@ -22806,7 +22826,7 @@
       </c>
     </row>
     <row r="150" spans="1:11">
-      <c r="A150" s="90" t="s">
+      <c r="A150" s="89" t="s">
         <v>9</v>
       </c>
       <c r="B150" s="48">
@@ -22840,7 +22860,7 @@
       </c>
     </row>
     <row r="151" spans="1:11">
-      <c r="A151" s="90" t="s">
+      <c r="A151" s="89" t="s">
         <v>298</v>
       </c>
       <c r="B151" s="48">
@@ -22911,7 +22931,7 @@
       </c>
     </row>
     <row r="153" spans="1:11">
-      <c r="A153" s="90" t="s">
+      <c r="A153" s="89" t="s">
         <v>304</v>
       </c>
       <c r="B153" s="48">
@@ -22945,7 +22965,7 @@
       </c>
     </row>
     <row r="154" spans="1:11">
-      <c r="A154" s="90" t="s">
+      <c r="A154" s="89" t="s">
         <v>305</v>
       </c>
       <c r="B154" s="48">
@@ -23016,7 +23036,7 @@
       </c>
     </row>
     <row r="156" spans="1:11">
-      <c r="A156" s="90" t="s">
+      <c r="A156" s="89" t="s">
         <v>310</v>
       </c>
       <c r="B156" s="48">
@@ -23087,7 +23107,7 @@
       </c>
     </row>
     <row r="158" spans="1:11">
-      <c r="A158" s="90" t="s">
+      <c r="A158" s="89" t="s">
         <v>313</v>
       </c>
       <c r="B158" s="48">
@@ -23158,7 +23178,7 @@
       </c>
     </row>
     <row r="160" spans="1:11">
-      <c r="A160" s="90" t="s">
+      <c r="A160" s="89" t="s">
         <v>315</v>
       </c>
       <c r="B160" s="48">
@@ -23229,7 +23249,7 @@
       </c>
     </row>
     <row r="162" spans="1:11">
-      <c r="A162" s="90" t="s">
+      <c r="A162" s="89" t="s">
         <v>319</v>
       </c>
       <c r="B162" s="48">
@@ -23263,7 +23283,7 @@
       </c>
     </row>
     <row r="163" spans="1:11">
-      <c r="A163" s="90" t="s">
+      <c r="A163" s="89" t="s">
         <v>320</v>
       </c>
       <c r="B163" s="48">
@@ -23297,7 +23317,7 @@
       </c>
     </row>
     <row r="164" spans="1:11">
-      <c r="A164" s="90" t="s">
+      <c r="A164" s="89" t="s">
         <v>321</v>
       </c>
       <c r="B164" s="48">
@@ -23328,7 +23348,7 @@
       </c>
     </row>
     <row r="165" spans="1:11">
-      <c r="A165" s="90" t="s">
+      <c r="A165" s="89" t="s">
         <v>324</v>
       </c>
       <c r="B165" s="48">
@@ -23362,7 +23382,7 @@
       </c>
     </row>
     <row r="166" spans="1:11">
-      <c r="A166" s="90" t="s">
+      <c r="A166" s="89" t="s">
         <v>325</v>
       </c>
       <c r="B166" s="48">
@@ -23396,7 +23416,7 @@
       </c>
     </row>
     <row r="167" spans="1:11">
-      <c r="A167" s="90" t="s">
+      <c r="A167" s="89" t="s">
         <v>328</v>
       </c>
       <c r="B167" s="48">
@@ -23560,7 +23580,7 @@
       </c>
     </row>
     <row r="172" spans="1:11">
-      <c r="A172" s="90" t="s">
+      <c r="A172" s="89" t="s">
         <v>336</v>
       </c>
       <c r="B172" s="48">
@@ -23593,7 +23613,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="173" spans="1:11">
+    <row r="173" ht="30" spans="1:11">
       <c r="A173" s="59" t="s">
         <v>337</v>
       </c>
@@ -23667,7 +23687,7 @@
         <v>3575</v>
       </c>
     </row>
-    <row r="175" ht="30" spans="1:11">
+    <row r="175" ht="45" spans="1:11">
       <c r="A175" s="58" t="s">
         <v>342</v>
       </c>
@@ -23852,7 +23872,7 @@
         <v>8575</v>
       </c>
     </row>
-    <row r="180" spans="1:11">
+    <row r="180" ht="30" spans="1:11">
       <c r="A180" s="58" t="s">
         <v>351</v>
       </c>
@@ -23889,7 +23909,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="181" spans="1:11">
+    <row r="181" ht="30" spans="1:11">
       <c r="A181" s="58" t="s">
         <v>352</v>
       </c>
@@ -23926,7 +23946,7 @@
         <v>2575</v>
       </c>
     </row>
-    <row r="182" ht="30" spans="1:11">
+    <row r="182" ht="45" spans="1:11">
       <c r="A182" s="58" t="s">
         <v>353</v>
       </c>
@@ -24111,7 +24131,7 @@
         <v>2575</v>
       </c>
     </row>
-    <row r="187" ht="30" spans="1:11">
+    <row r="187" ht="45" spans="1:11">
       <c r="A187" s="59" t="s">
         <v>361</v>
       </c>
@@ -24185,7 +24205,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="189" spans="1:11">
+    <row r="189" ht="30" spans="1:11">
       <c r="A189" s="58" t="s">
         <v>363</v>
       </c>
@@ -24293,7 +24313,7 @@
         <v>8575</v>
       </c>
     </row>
-    <row r="192" spans="1:11">
+    <row r="192" ht="30" spans="1:11">
       <c r="A192" s="58" t="s">
         <v>366</v>
       </c>
@@ -24612,7 +24632,7 @@
       <c r="C201" t="s">
         <v>120</v>
       </c>
-      <c r="D201" s="91" t="s">
+      <c r="D201" s="90" t="s">
         <v>378</v>
       </c>
       <c r="F201" s="18">
@@ -24837,7 +24857,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="208" ht="54" spans="1:11">
+    <row r="208" ht="67.5" spans="1:11">
       <c r="A208" s="58" t="s">
         <v>387</v>
       </c>
@@ -25180,7 +25200,7 @@
         <v>2975</v>
       </c>
     </row>
-    <row r="218" spans="1:11">
+    <row r="218" ht="30" spans="1:11">
       <c r="A218" s="58" t="s">
         <v>398</v>
       </c>
@@ -25254,7 +25274,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="220" spans="1:11">
+    <row r="220" ht="30" spans="1:11">
       <c r="A220" s="58" t="s">
         <v>404</v>
       </c>
@@ -25291,7 +25311,7 @@
         <v>8575</v>
       </c>
     </row>
-    <row r="221" ht="30" spans="1:11">
+    <row r="221" ht="45" spans="1:11">
       <c r="A221" s="59" t="s">
         <v>405</v>
       </c>
@@ -25328,7 +25348,7 @@
         <v>3575</v>
       </c>
     </row>
-    <row r="222" ht="30" spans="1:11">
+    <row r="222" ht="45" spans="1:11">
       <c r="A222" s="59" t="s">
         <v>409</v>
       </c>
@@ -25399,7 +25419,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="224" ht="45" spans="1:11">
+    <row r="224" ht="60" spans="1:11">
       <c r="A224" s="14" t="s">
         <v>414</v>
       </c>
@@ -26024,7 +26044,7 @@
       <c r="C242" t="s">
         <v>454</v>
       </c>
-      <c r="D242" s="91" t="s">
+      <c r="D242" s="90" t="s">
         <v>378</v>
       </c>
       <c r="F242" s="18">
@@ -26462,7 +26482,7 @@
         <v>3575</v>
       </c>
     </row>
-    <row r="255" ht="30" spans="1:11">
+    <row r="255" ht="45" spans="1:11">
       <c r="A255" s="63" t="s">
         <v>472</v>
       </c>
@@ -26533,7 +26553,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="257" spans="1:11">
+    <row r="257" ht="30" spans="1:11">
       <c r="A257" s="63" t="s">
         <v>474</v>
       </c>
@@ -26703,7 +26723,7 @@
         <v>8575</v>
       </c>
     </row>
-    <row r="262" spans="1:11">
+    <row r="262" ht="30" spans="1:11">
       <c r="A262" s="63" t="s">
         <v>478</v>
       </c>
@@ -26805,7 +26825,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="265" ht="45" spans="1:11">
+    <row r="265" ht="60" spans="1:11">
       <c r="A265" s="62" t="s">
         <v>481</v>
       </c>
@@ -27034,7 +27054,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="272" spans="1:11">
+    <row r="272" ht="30" spans="1:11">
       <c r="A272" s="62" t="s">
         <v>490</v>
       </c>
@@ -27139,7 +27159,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="275" spans="1:11">
+    <row r="275" ht="30" spans="1:11">
       <c r="A275" s="63" t="s">
         <v>494</v>
       </c>
@@ -27173,7 +27193,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="276" spans="1:11">
+    <row r="276" ht="30" spans="1:11">
       <c r="A276" s="63" t="s">
         <v>495</v>
       </c>
@@ -27207,7 +27227,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="277" spans="1:11">
+    <row r="277" ht="30" spans="1:11">
       <c r="A277" s="62" t="s">
         <v>496</v>
       </c>
@@ -27371,7 +27391,7 @@
         <v>3575</v>
       </c>
     </row>
-    <row r="282" ht="30" spans="1:11">
+    <row r="282" ht="45" spans="1:11">
       <c r="A282" s="62" t="s">
         <v>507</v>
       </c>
@@ -27501,7 +27521,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="286" spans="1:11">
+    <row r="286" ht="27" spans="1:11">
       <c r="A286" s="62" t="s">
         <v>511</v>
       </c>
@@ -27569,7 +27589,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="288" spans="1:11">
+    <row r="288" ht="30" spans="1:11">
       <c r="A288" s="63" t="s">
         <v>516</v>
       </c>
@@ -27684,7 +27704,7 @@
       <c r="C291" t="s">
         <v>35</v>
       </c>
-      <c r="D291" s="91" t="s">
+      <c r="D291" s="90" t="s">
         <v>155</v>
       </c>
       <c r="E291" t="s">
@@ -27776,7 +27796,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="294" spans="1:11">
+    <row r="294" ht="27" spans="1:11">
       <c r="A294" s="62" t="s">
         <v>511</v>
       </c>
@@ -27878,7 +27898,7 @@
         <v>6425</v>
       </c>
     </row>
-    <row r="297" spans="1:11">
+    <row r="297" ht="30" spans="1:11">
       <c r="A297" s="62" t="s">
         <v>522</v>
       </c>
@@ -27949,7 +27969,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="299" ht="30" spans="1:11">
+    <row r="299" ht="45" spans="1:11">
       <c r="A299" s="62" t="s">
         <v>525</v>
       </c>
@@ -27993,7 +28013,7 @@
       <c r="C300" t="s">
         <v>454</v>
       </c>
-      <c r="D300" s="91" t="s">
+      <c r="D300" s="90" t="s">
         <v>378</v>
       </c>
       <c r="F300" s="18">
@@ -28014,7 +28034,7 @@
         <v>3450</v>
       </c>
     </row>
-    <row r="301" ht="30" spans="1:11">
+    <row r="301" ht="45" spans="1:11">
       <c r="A301" s="62" t="s">
         <v>527</v>
       </c>
@@ -28119,7 +28139,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="304" ht="45" spans="1:11">
+    <row r="304" ht="60" spans="1:11">
       <c r="A304" s="62" t="s">
         <v>531</v>
       </c>
@@ -28193,7 +28213,7 @@
         <v>8575</v>
       </c>
     </row>
-    <row r="306" spans="1:11">
+    <row r="306" ht="30" spans="1:11">
       <c r="A306" s="62" t="s">
         <v>533</v>
       </c>
@@ -28338,7 +28358,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="310" spans="1:11">
+    <row r="310" ht="30" spans="1:11">
       <c r="A310" s="63" t="s">
         <v>540</v>
       </c>
@@ -28895,7 +28915,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="326" spans="1:11">
+    <row r="326" ht="30" spans="1:11">
       <c r="A326" s="62" t="s">
         <v>566</v>
       </c>
@@ -29254,7 +29274,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="337" spans="1:11">
+    <row r="337" ht="30" spans="1:11">
       <c r="A337" s="63" t="s">
         <v>584</v>
       </c>
@@ -29452,7 +29472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:11">
+    <row r="343" ht="30" spans="1:11">
       <c r="A343" s="62" t="s">
         <v>591</v>
       </c>
@@ -29557,7 +29577,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="346" ht="30" spans="1:11">
+    <row r="346" ht="45" spans="1:11">
       <c r="A346" s="62" t="s">
         <v>596</v>
       </c>
@@ -29594,7 +29614,7 @@
         <v>10500</v>
       </c>
     </row>
-    <row r="347" ht="45" spans="1:11">
+    <row r="347" ht="60" spans="1:11">
       <c r="A347" s="62" t="s">
         <v>597</v>
       </c>
@@ -29770,7 +29790,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="352" spans="1:11">
+    <row r="352" ht="30" spans="1:11">
       <c r="A352" s="62" t="s">
         <v>602</v>
       </c>
@@ -29844,7 +29864,7 @@
         <v>8575</v>
       </c>
     </row>
-    <row r="354" spans="1:11">
+    <row r="354" ht="30" spans="1:11">
       <c r="A354" s="62" t="s">
         <v>604</v>
       </c>
@@ -29949,7 +29969,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="357" spans="1:11">
+    <row r="357" ht="30" spans="1:11">
       <c r="A357" s="62" t="s">
         <v>610</v>
       </c>
@@ -29983,7 +30003,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="358" spans="1:11">
+    <row r="358" ht="30" spans="1:11">
       <c r="A358" s="62" t="s">
         <v>611</v>
       </c>
@@ -30020,7 +30040,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="359" spans="1:11">
+    <row r="359" ht="30" spans="1:11">
       <c r="A359" s="62" t="s">
         <v>612</v>
       </c>
@@ -30094,7 +30114,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="361" ht="30" spans="1:11">
+    <row r="361" ht="45" spans="1:11">
       <c r="A361" s="62" t="s">
         <v>617</v>
       </c>
@@ -30166,7 +30186,7 @@
         <v>5250</v>
       </c>
     </row>
-    <row r="363" spans="1:11">
+    <row r="363" ht="30" spans="1:11">
       <c r="A363" s="62" t="s">
         <v>612</v>
       </c>
@@ -30240,7 +30260,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="365" ht="30" spans="1:11">
+    <row r="365" ht="45" spans="1:11">
       <c r="A365" s="62" t="s">
         <v>617</v>
       </c>
@@ -30345,7 +30365,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="368" ht="30" spans="1:11">
+    <row r="368" ht="45" spans="1:11">
       <c r="A368" s="62" t="s">
         <v>624</v>
       </c>
@@ -30419,7 +30439,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="370" ht="45" spans="1:11">
+    <row r="370" ht="60" spans="1:11">
       <c r="A370" s="62" t="s">
         <v>627</v>
       </c>
@@ -30669,7 +30689,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="377" spans="1:11">
+    <row r="377" ht="30" spans="1:11">
       <c r="A377" s="62" t="s">
         <v>635</v>
       </c>
@@ -30706,7 +30726,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="378" ht="30" spans="1:11">
+    <row r="378" ht="45" spans="1:11">
       <c r="A378" s="62" t="s">
         <v>636</v>
       </c>
@@ -30780,7 +30800,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="380" spans="1:11">
+    <row r="380" ht="30" spans="1:11">
       <c r="A380" s="63" t="s">
         <v>638</v>
       </c>
@@ -30817,7 +30837,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="381" spans="1:11">
+    <row r="381" ht="30" spans="1:11">
       <c r="A381" s="62" t="s">
         <v>639</v>
       </c>
@@ -30990,7 +31010,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="386" ht="30" spans="1:11">
+    <row r="386" ht="45" spans="1:11">
       <c r="A386" s="62" t="s">
         <v>644</v>
       </c>
@@ -31132,7 +31152,7 @@
         <v>2440</v>
       </c>
     </row>
-    <row r="390" spans="1:11">
+    <row r="390" ht="30" spans="1:11">
       <c r="A390" s="62" t="s">
         <v>649</v>
       </c>
@@ -31206,7 +31226,7 @@
         <v>1932.5</v>
       </c>
     </row>
-    <row r="392" spans="1:11">
+    <row r="392" ht="30" spans="1:11">
       <c r="A392" s="62" t="s">
         <v>653</v>
       </c>
@@ -31305,7 +31325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" ht="30" spans="1:11">
+    <row r="395" ht="45" spans="1:11">
       <c r="A395" s="62" t="s">
         <v>658</v>
       </c>
@@ -31450,7 +31470,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="399" spans="1:11">
+    <row r="399" ht="30" spans="1:11">
       <c r="A399" s="62" t="s">
         <v>665</v>
       </c>
@@ -31731,7 +31751,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="407" spans="1:11">
+    <row r="407" ht="30" spans="1:11">
       <c r="A407" s="62" t="s">
         <v>673</v>
       </c>
@@ -31907,7 +31927,7 @@
         <v>3575</v>
       </c>
     </row>
-    <row r="412" ht="15.75" spans="1:11">
+    <row r="412" ht="30.75" spans="1:11">
       <c r="A412" s="63" t="s">
         <v>678</v>
       </c>
@@ -31944,7 +31964,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="413" spans="1:11">
+    <row r="413" ht="27" spans="1:11">
       <c r="A413" s="63" t="s">
         <v>679</v>
       </c>
@@ -32089,7 +32109,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="417" spans="1:11">
+    <row r="417" ht="30" spans="1:11">
       <c r="A417" s="62" t="s">
         <v>686</v>
       </c>
@@ -32231,7 +32251,7 @@
         <v>3575</v>
       </c>
     </row>
-    <row r="421" spans="1:11">
+    <row r="421" ht="30" spans="1:11">
       <c r="A421" s="63" t="s">
         <v>689</v>
       </c>
@@ -32447,7 +32467,7 @@
         <v>5350</v>
       </c>
     </row>
-    <row r="427" ht="30" spans="1:11">
+    <row r="427" ht="45" spans="1:11">
       <c r="A427" s="62" t="s">
         <v>696</v>
       </c>
@@ -32657,7 +32677,7 @@
         <v>5250</v>
       </c>
     </row>
-    <row r="433" spans="1:11">
+    <row r="433" ht="30" spans="1:11">
       <c r="A433" s="63" t="s">
         <v>703</v>
       </c>
@@ -33083,7 +33103,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="445" ht="45" spans="1:11">
+    <row r="445" ht="60" spans="1:11">
       <c r="A445" s="62" t="s">
         <v>718</v>
       </c>
@@ -33228,7 +33248,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="449" ht="30" spans="1:11">
+    <row r="449" ht="45" spans="1:11">
       <c r="A449" s="62" t="s">
         <v>723</v>
       </c>
@@ -33333,7 +33353,7 @@
         <v>12200</v>
       </c>
     </row>
-    <row r="452" spans="1:11">
+    <row r="452" ht="30" spans="1:11">
       <c r="A452" s="62" t="s">
         <v>729</v>
       </c>
@@ -33404,7 +33424,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="454" spans="1:11">
+    <row r="454" ht="30" spans="1:11">
       <c r="A454" s="62" t="s">
         <v>731</v>
       </c>
@@ -33441,7 +33461,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="455" spans="1:11">
+    <row r="455" ht="30" spans="1:11">
       <c r="A455" s="62" t="s">
         <v>732</v>
       </c>
@@ -33858,7 +33878,7 @@
         <v>3575</v>
       </c>
     </row>
-    <row r="467" spans="1:11">
+    <row r="467" ht="30" spans="1:11">
       <c r="A467" s="62" t="s">
         <v>746</v>
       </c>
@@ -33895,7 +33915,7 @@
         <v>2432.5</v>
       </c>
     </row>
-    <row r="468" ht="45" spans="1:11">
+    <row r="468" ht="60" spans="1:11">
       <c r="A468" s="63" t="s">
         <v>747</v>
       </c>
@@ -34222,7 +34242,7 @@
         <v>5250</v>
       </c>
     </row>
-    <row r="477" spans="1:11">
+    <row r="477" ht="30" spans="1:11">
       <c r="A477" s="62" t="s">
         <v>757</v>
       </c>
@@ -34293,7 +34313,7 @@
         <v>2575</v>
       </c>
     </row>
-    <row r="479" spans="1:11">
+    <row r="479" ht="30" spans="1:11">
       <c r="A479" s="62" t="s">
         <v>759</v>
       </c>
@@ -34673,7 +34693,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="490" spans="1:11">
+    <row r="490" ht="30" spans="1:11">
       <c r="A490" s="62" t="s">
         <v>773</v>
       </c>
@@ -34741,7 +34761,7 @@
         <v>2690</v>
       </c>
     </row>
-    <row r="492" ht="45" spans="1:11">
+    <row r="492" ht="60" spans="1:11">
       <c r="A492" s="62" t="s">
         <v>774</v>
       </c>
@@ -34923,7 +34943,7 @@
         <v>5250</v>
       </c>
     </row>
-    <row r="497" spans="1:11">
+    <row r="497" ht="30" spans="1:11">
       <c r="A497" s="63" t="s">
         <v>779</v>
       </c>
@@ -34957,7 +34977,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="498" spans="1:11">
+    <row r="498" ht="30" spans="1:11">
       <c r="A498" s="62" t="s">
         <v>780</v>
       </c>
@@ -35253,7 +35273,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="506" spans="1:11">
+    <row r="506" ht="27" spans="1:11">
       <c r="A506" s="62" t="s">
         <v>790</v>
       </c>
@@ -35361,7 +35381,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="509" spans="1:11">
+    <row r="509" ht="30" spans="1:11">
       <c r="A509" s="62" t="s">
         <v>793</v>
       </c>
@@ -35398,7 +35418,7 @@
         <v>2432.5</v>
       </c>
     </row>
-    <row r="510" ht="30" spans="1:11">
+    <row r="510" ht="45" spans="1:11">
       <c r="A510" s="62" t="s">
         <v>794</v>
       </c>
@@ -35720,7 +35740,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="519" spans="1:11">
+    <row r="519" ht="30" spans="1:11">
       <c r="A519" s="62" t="s">
         <v>806</v>
       </c>
@@ -35757,7 +35777,7 @@
         <v>932.5</v>
       </c>
     </row>
-    <row r="520" ht="30" spans="1:11">
+    <row r="520" ht="45" spans="1:11">
       <c r="A520" s="62" t="s">
         <v>807</v>
       </c>
@@ -36103,7 +36123,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="530" ht="45" spans="1:11">
+    <row r="530" ht="60" spans="1:11">
       <c r="A530" s="62" t="s">
         <v>818</v>
       </c>
@@ -36385,7 +36405,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="538" spans="1:11">
+    <row r="538" ht="30" spans="1:11">
       <c r="A538" s="62" t="s">
         <v>827</v>
       </c>
@@ -36657,7 +36677,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="546" spans="1:11">
+    <row r="546" ht="30" spans="1:11">
       <c r="A546" s="62" t="s">
         <v>835</v>
       </c>
@@ -36836,7 +36856,7 @@
         <v>3480.75</v>
       </c>
     </row>
-    <row r="551" spans="1:11">
+    <row r="551" ht="30" spans="1:11">
       <c r="A551" s="62" t="s">
         <v>843</v>
       </c>
@@ -36975,7 +36995,7 @@
         <v>8925</v>
       </c>
     </row>
-    <row r="555" spans="1:11">
+    <row r="555" ht="30" spans="1:11">
       <c r="A555" s="62" t="s">
         <v>853</v>
       </c>
@@ -37012,7 +37032,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="556" spans="1:11">
+    <row r="556" ht="30" spans="1:11">
       <c r="A556" s="62" t="s">
         <v>854</v>
       </c>
@@ -37120,7 +37140,7 @@
         <v>20575</v>
       </c>
     </row>
-    <row r="559" spans="1:11">
+    <row r="559" ht="30" spans="1:11">
       <c r="A559" s="62" t="s">
         <v>857</v>
       </c>
@@ -37241,7 +37261,7 @@
       <c r="C562" t="s">
         <v>866</v>
       </c>
-      <c r="D562" s="91" t="s">
+      <c r="D562" s="90" t="s">
         <v>867</v>
       </c>
       <c r="E562" s="41" t="s">
@@ -37299,7 +37319,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="564" ht="30" spans="1:11">
+    <row r="564" ht="45" spans="1:11">
       <c r="A564" s="63" t="s">
         <v>870</v>
       </c>
@@ -37577,7 +37597,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="572" spans="1:11">
+    <row r="572" ht="30" spans="1:11">
       <c r="A572" s="62" t="s">
         <v>880</v>
       </c>
@@ -37756,7 +37776,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="577" ht="45" spans="1:11">
+    <row r="577" ht="60" spans="1:11">
       <c r="A577" s="63" t="s">
         <v>886</v>
       </c>
@@ -37852,7 +37872,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="580" spans="1:11">
+    <row r="580" ht="30" spans="1:11">
       <c r="A580" s="62" t="s">
         <v>889</v>
       </c>
@@ -37889,7 +37909,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="581" ht="30" spans="1:11">
+    <row r="581" ht="45" spans="1:11">
       <c r="A581" s="62" t="s">
         <v>890</v>
       </c>
@@ -38139,7 +38159,7 @@
         <v>1932.5</v>
       </c>
     </row>
-    <row r="588" ht="30" spans="1:11">
+    <row r="588" ht="45" spans="1:11">
       <c r="A588" s="63" t="s">
         <v>899</v>
       </c>
@@ -38173,7 +38193,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="589" spans="1:11">
+    <row r="589" ht="30" spans="1:11">
       <c r="A589" s="63" t="s">
         <v>900</v>
       </c>
@@ -38244,7 +38264,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="591" ht="30" spans="1:11">
+    <row r="591" ht="45" spans="1:11">
       <c r="A591" s="62" t="s">
         <v>901</v>
       </c>
@@ -38565,7 +38585,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="600" ht="45.75" spans="1:11">
+    <row r="600" ht="60.75" spans="1:11">
       <c r="A600" s="62" t="s">
         <v>910</v>
       </c>
@@ -38599,7 +38619,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="601" ht="27" spans="1:11">
+    <row r="601" ht="40.5" spans="1:11">
       <c r="A601" s="62" t="s">
         <v>911</v>
       </c>
@@ -38917,7 +38937,7 @@
         <v>2225</v>
       </c>
     </row>
-    <row r="610" spans="1:11">
+    <row r="610" ht="27" spans="1:11">
       <c r="A610" s="62" t="s">
         <v>924</v>
       </c>
@@ -39028,7 +39048,7 @@
         <v>1932.5</v>
       </c>
     </row>
-    <row r="613" spans="1:11">
+    <row r="613" ht="30" spans="1:11">
       <c r="A613" s="62" t="s">
         <v>928</v>
       </c>
@@ -39250,7 +39270,7 @@
         <v>1932.5</v>
       </c>
     </row>
-    <row r="619" spans="1:11">
+    <row r="619" ht="30" spans="1:11">
       <c r="A619" s="62" t="s">
         <v>936</v>
       </c>
@@ -39324,7 +39344,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="621" ht="30.75" spans="1:11">
+    <row r="621" ht="45.75" spans="1:11">
       <c r="A621" s="63" t="s">
         <v>938</v>
       </c>
@@ -39361,7 +39381,7 @@
         <v>5075</v>
       </c>
     </row>
-    <row r="622" ht="27" spans="1:11">
+    <row r="622" ht="40.5" spans="1:11">
       <c r="A622" s="62" t="s">
         <v>939</v>
       </c>
@@ -39544,7 +39564,7 @@
       </c>
     </row>
     <row r="627" ht="30" spans="1:11">
-      <c r="A627" s="73" t="s">
+      <c r="A627" s="62" t="s">
         <v>944</v>
       </c>
       <c r="B627" s="48">
@@ -39581,7 +39601,7 @@
       </c>
     </row>
     <row r="628" spans="1:11">
-      <c r="A628" s="74" t="s">
+      <c r="A628" s="63" t="s">
         <v>945</v>
       </c>
       <c r="B628" s="48">
@@ -39615,7 +39635,7 @@
       </c>
     </row>
     <row r="629" spans="1:11">
-      <c r="A629" s="73" t="s">
+      <c r="A629" s="62" t="s">
         <v>946</v>
       </c>
       <c r="B629" s="48">
@@ -39649,7 +39669,7 @@
       </c>
     </row>
     <row r="630" ht="45" spans="1:11">
-      <c r="A630" s="73" t="s">
+      <c r="A630" s="62" t="s">
         <v>947</v>
       </c>
       <c r="B630" s="48">
@@ -39685,8 +39705,8 @@
         <v>5750</v>
       </c>
     </row>
-    <row r="631" ht="30" spans="1:11">
-      <c r="A631" s="73" t="s">
+    <row r="631" ht="45" spans="1:11">
+      <c r="A631" s="62" t="s">
         <v>948</v>
       </c>
       <c r="B631" s="48">
@@ -39722,8 +39742,8 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="632" spans="1:11">
-      <c r="A632" s="74" t="s">
+    <row r="632" ht="30" spans="1:11">
+      <c r="A632" s="63" t="s">
         <v>949</v>
       </c>
       <c r="B632" s="48">
@@ -39759,8 +39779,8 @@
         <v>2575</v>
       </c>
     </row>
-    <row r="633" ht="30" spans="1:11">
-      <c r="A633" s="73" t="s">
+    <row r="633" ht="45" spans="1:11">
+      <c r="A633" s="62" t="s">
         <v>950</v>
       </c>
       <c r="B633" s="48">
@@ -39796,47 +39816,158 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="634" spans="10:11">
+    <row r="634" ht="30" spans="1:11">
+      <c r="A634" s="73" t="s">
+        <v>951</v>
+      </c>
+      <c r="B634" s="48">
+        <v>42973</v>
+      </c>
+      <c r="C634" t="s">
+        <v>46</v>
+      </c>
+      <c r="D634" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="E634" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="F634" s="18">
+        <v>51500</v>
+      </c>
+      <c r="G634" t="s">
+        <v>16</v>
+      </c>
+      <c r="H634" s="18">
+        <v>51500</v>
+      </c>
+      <c r="I634" s="18">
+        <v>51500</v>
+      </c>
       <c r="J634">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>2575</v>
       </c>
       <c r="K634" s="18">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="635" spans="10:11">
+        <v>2575</v>
+      </c>
+    </row>
+    <row r="635" ht="30" spans="1:11">
+      <c r="A635" s="73" t="s">
+        <v>952</v>
+      </c>
+      <c r="B635" s="48">
+        <v>42973</v>
+      </c>
+      <c r="C635" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="D635" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="E635" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="F635" s="19">
+        <v>100000</v>
+      </c>
+      <c r="G635" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="H635" s="19">
+        <v>102500</v>
+      </c>
+      <c r="I635" s="19">
+        <v>100000</v>
+      </c>
       <c r="J635">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>5125</v>
       </c>
       <c r="K635" s="18">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="636" spans="10:11">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="636" spans="1:11">
+      <c r="A636" s="73" t="s">
+        <v>953</v>
+      </c>
+      <c r="B636" s="48">
+        <v>42973</v>
+      </c>
+      <c r="C636" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="D636" s="54" t="s">
+        <v>207</v>
+      </c>
+      <c r="F636" s="18">
+        <v>26000</v>
+      </c>
+      <c r="G636" t="s">
+        <v>13</v>
+      </c>
+      <c r="H636" s="18">
+        <v>25000</v>
+      </c>
+      <c r="I636" s="18">
+        <v>26000</v>
+      </c>
       <c r="J636">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>1250</v>
       </c>
       <c r="K636" s="18">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="637" spans="10:11">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="637" spans="1:11">
+      <c r="A637" s="73" t="s">
+        <v>954</v>
+      </c>
+      <c r="B637" s="48">
+        <v>42973</v>
+      </c>
+      <c r="C637" t="s">
+        <v>159</v>
+      </c>
+      <c r="D637" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="E637" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="F637" s="19">
+        <v>50000</v>
+      </c>
+      <c r="G637" t="s">
+        <v>16</v>
+      </c>
+      <c r="H637" s="19">
+        <v>51650</v>
+      </c>
+      <c r="I637" s="19">
+        <v>51500</v>
+      </c>
       <c r="J637">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>2582.5</v>
       </c>
       <c r="K637" s="18">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="638" spans="10:11">
+        <v>932.5</v>
+      </c>
+    </row>
+    <row r="638" spans="1:11">
+      <c r="A638" s="73" t="s">
+        <v>955</v>
+      </c>
+      <c r="B638" s="48">
+        <v>42973</v>
+      </c>
       <c r="J638">
         <f t="shared" si="26"/>
         <v>0</v>
@@ -39846,7 +39977,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="639" spans="10:11">
+    <row r="639" spans="1:11">
+      <c r="A639" s="73" t="s">
+        <v>956</v>
+      </c>
+      <c r="B639" s="48">
+        <v>42973</v>
+      </c>
       <c r="J639">
         <f t="shared" si="26"/>
         <v>0</v>
@@ -39856,7 +39993,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="640" spans="10:11">
+    <row r="640" spans="1:11">
+      <c r="A640" s="73" t="s">
+        <v>957</v>
+      </c>
+      <c r="B640" s="48">
+        <v>42973</v>
+      </c>
       <c r="J640">
         <f t="shared" si="26"/>
         <v>0</v>
@@ -39897,7 +40040,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:I626"/>
+  <autoFilter ref="B1:I633"/>
   <hyperlinks>
     <hyperlink ref="A173" r:id="rId1" display="BL171111JKC7ELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/795416"/>
     <hyperlink ref="A174" r:id="rId2" display="BL171111JMU2ELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/798491"/>
@@ -40350,6 +40493,13 @@
     <hyperlink ref="A631" r:id="rId440" display="BL171114SV2NELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/5696307"/>
     <hyperlink ref="A632" r:id="rId441" display="BL171114SV33ELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/5696322"/>
     <hyperlink ref="A633" r:id="rId442" display="BL171114TI8MELC " tooltip="https://www.bukalapak.com/payment/electricity/transactions/5723466"/>
+    <hyperlink ref="A634" r:id="rId443" display="BL171114TRVXELC " tooltip="https://www.bukalapak.com/payment/electricity/transactions/5735307"/>
+    <hyperlink ref="A635" r:id="rId444" display="BL171114U1Y8ELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/5746412"/>
+    <hyperlink ref="A636" r:id="rId445" display="BL17114EY4AIINV" tooltip="https://www.bukalapak.com/payment/invoices/178492632"/>
+    <hyperlink ref="A637" r:id="rId446" display="BL171114USZXELC " tooltip="https://www.bukalapak.com/payment/electricity/transactions/5779547"/>
+    <hyperlink ref="A638" r:id="rId447" display="BL171114UTB8ELC " tooltip="https://www.bukalapak.com/payment/electricity/transactions/5779907"/>
+    <hyperlink ref="A639" r:id="rId448" display="BL17114EYMOXINV" tooltip="https://www.bukalapak.com/payment/invoices/178515187"/>
+    <hyperlink ref="A640" r:id="rId449" display="BL171114UTISELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/5780172"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -40368,28 +40518,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="24.1416666666667" customWidth="1"/>
-    <col min="2" max="2" width="13.8583333333333" customWidth="1"/>
-    <col min="3" max="3" width="20.2833333333333" customWidth="1"/>
-    <col min="4" max="4" width="26.7166666666667" customWidth="1"/>
-    <col min="5" max="5" width="13.7166666666667" customWidth="1"/>
+    <col min="1" max="1" width="24.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="13.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="20.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="26.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="13.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="37" t="s">
-        <v>951</v>
+        <v>958</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>952</v>
+        <v>959</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>953</v>
+        <v>960</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>954</v>
+        <v>961</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>955</v>
+        <v>962</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -40666,7 +40816,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="27" t="s">
-        <v>956</v>
+        <v>963</v>
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
@@ -40678,7 +40828,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="38" t="s">
-        <v>957</v>
+        <v>964</v>
       </c>
       <c r="E20" s="39">
         <f>5%*E18</f>
@@ -40687,7 +40837,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="38" t="s">
-        <v>958</v>
+        <v>965</v>
       </c>
       <c r="E21" s="39">
         <f>10%*E18</f>
@@ -40714,32 +40864,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="11.575" customWidth="1"/>
-    <col min="2" max="2" width="15.2833333333333" customWidth="1"/>
+    <col min="1" max="1" width="11.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="15.2857142857143" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="20.2833333333333" customWidth="1"/>
+    <col min="4" max="4" width="20.2857142857143" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="14.1416666666667" customWidth="1"/>
+    <col min="6" max="6" width="14.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="21" t="s">
-        <v>959</v>
+        <v>966</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>960</v>
+        <v>967</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>961</v>
+        <v>968</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>31</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>962</v>
+        <v>969</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -40818,7 +40968,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="27" t="s">
-        <v>963</v>
+        <v>970</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
@@ -40831,7 +40981,7 @@
     </row>
     <row r="9" spans="4:5">
       <c r="D9" s="10" t="s">
-        <v>964</v>
+        <v>971</v>
       </c>
       <c r="E9" s="31">
         <v>1000000</v>
@@ -40839,7 +40989,7 @@
     </row>
     <row r="10" spans="4:5">
       <c r="D10" s="3" t="s">
-        <v>965</v>
+        <v>972</v>
       </c>
       <c r="E10" s="25">
         <f>E9-E6</f>
@@ -40852,7 +41002,7 @@
     </row>
     <row r="12" spans="4:5">
       <c r="D12" s="23" t="s">
-        <v>966</v>
+        <v>973</v>
       </c>
       <c r="E12" s="25">
         <v>300000</v>
@@ -40860,7 +41010,7 @@
     </row>
     <row r="13" spans="4:5">
       <c r="D13" s="3" t="s">
-        <v>967</v>
+        <v>974</v>
       </c>
       <c r="E13" s="25">
         <v>300000</v>
@@ -40868,7 +41018,7 @@
     </row>
     <row r="14" spans="4:5">
       <c r="D14" s="10" t="s">
-        <v>968</v>
+        <v>975</v>
       </c>
       <c r="E14" s="31">
         <f>E13+E12</f>
@@ -40881,7 +41031,7 @@
     </row>
     <row r="16" spans="4:5">
       <c r="D16" s="10" t="s">
-        <v>969</v>
+        <v>976</v>
       </c>
       <c r="E16" s="31">
         <f>E10-E14</f>
@@ -41116,7 +41266,7 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="34" t="s">
-        <v>963</v>
+        <v>970</v>
       </c>
       <c r="B32" s="35"/>
       <c r="C32" s="35"/>
@@ -41129,7 +41279,7 @@
     </row>
     <row r="34" spans="4:5">
       <c r="D34" s="10" t="s">
-        <v>970</v>
+        <v>977</v>
       </c>
       <c r="E34" s="13">
         <f>E16</f>
@@ -41146,7 +41296,7 @@
     </row>
     <row r="36" spans="4:5">
       <c r="D36" s="10" t="s">
-        <v>971</v>
+        <v>978</v>
       </c>
       <c r="E36" s="13">
         <f>E34+E35</f>
@@ -41159,7 +41309,7 @@
     </row>
     <row r="38" spans="4:5">
       <c r="D38" s="10" t="s">
-        <v>972</v>
+        <v>979</v>
       </c>
       <c r="E38" s="13">
         <f>E36-E32</f>
@@ -41186,17 +41336,17 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.2833333333333" customWidth="1"/>
+    <col min="1" max="1" width="21.2857142857143" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="18.575" customWidth="1"/>
+    <col min="3" max="3" width="18.5714285714286" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="10.425" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11.2833333333333" customWidth="1"/>
-    <col min="7" max="7" width="6.85833333333333" customWidth="1"/>
+    <col min="5" max="5" width="10.4285714285714" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.2857142857143" customWidth="1"/>
+    <col min="7" max="7" width="6.85714285714286" customWidth="1"/>
     <col min="8" max="8" width="9" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="21.8583333333333" customWidth="1"/>
+    <col min="9" max="9" width="21.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -41254,7 +41404,7 @@
         <v>205000</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>973</v>
+        <v>980</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -41283,7 +41433,7 @@
         <v>205000</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>973</v>
+        <v>980</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -41312,7 +41462,7 @@
         <v>205000</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>973</v>
+        <v>980</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:9">
@@ -41341,7 +41491,7 @@
         <v>11300</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>973</v>
+        <v>980</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -41370,11 +41520,11 @@
         <v>201500</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>974</v>
+        <v>981</v>
       </c>
     </row>
     <row r="7" ht="30" hidden="1" spans="1:9">
-      <c r="A7" s="90" t="s">
+      <c r="A7" s="89" t="s">
         <v>261</v>
       </c>
       <c r="B7" s="15">
@@ -41448,7 +41598,7 @@
     </row>
     <row r="12" spans="4:9">
       <c r="D12" t="s">
-        <v>975</v>
+        <v>982</v>
       </c>
       <c r="I12" s="20">
         <v>695000</v>
@@ -41456,7 +41606,7 @@
     </row>
     <row r="13" spans="4:9">
       <c r="D13" t="s">
-        <v>976</v>
+        <v>983</v>
       </c>
       <c r="I13" s="20">
         <f>F2+F3+F4+F5</f>
@@ -41468,7 +41618,7 @@
     </row>
     <row r="15" spans="4:9">
       <c r="D15" t="s">
-        <v>972</v>
+        <v>979</v>
       </c>
       <c r="I15" s="20">
         <f>I12-I13</f>

</xml_diff>

<commit_message>
adm dana banin banat
</commit_message>
<xml_diff>
--- a/Jual Pulsa.xlsx
+++ b/Jual Pulsa.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Ustadz Fauzan" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$B$1:$I$633</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$B$1:$I$640</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <pivotCaches>
@@ -2983,13 +2983,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -3054,14 +3054,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3075,21 +3075,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -3098,71 +3083,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3190,10 +3112,88 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3224,13 +3224,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3242,19 +3254,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3284,7 +3290,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3296,49 +3350,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3356,55 +3386,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3607,6 +3607,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -3615,27 +3626,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3664,6 +3664,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -3672,29 +3687,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3706,134 +3706,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -3841,7 +3841,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3851,15 +3851,15 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3880,8 +3880,8 @@
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -3912,12 +3912,12 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3952,25 +3952,24 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
@@ -4057,10 +4056,10 @@
       <numFmt numFmtId="183" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="178" formatCode="d\-mmm\-yyyy;@"/>
@@ -4483,10 +4482,10 @@
       <numFmt numFmtId="187" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -5617,7 +5616,7 @@
         <s v="M. SYARIFUDDIN"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Harga" numFmtId="176">
+    <cacheField name="Harga" numFmtId="177">
       <sharedItems containsBlank="1" containsNumber="1" containsInteger="1" containsMixedTypes="1" count="52">
         <m/>
         <s v="Deposit"/>
@@ -5684,7 +5683,7 @@
         <s v="Listrik Pasca"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Nominal" numFmtId="176">
+    <cacheField name="Nominal" numFmtId="177">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="5000" maxValue="510000" count="61">
         <n v="57000"/>
         <n v="11000"/>
@@ -5749,7 +5748,7 @@
         <n v="78500"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Dibayar" numFmtId="176">
+    <cacheField name="Dibayar" numFmtId="177">
       <sharedItems containsBlank="1" containsNumber="1" containsInteger="1" containsMixedTypes="1" count="60">
         <n v="57000"/>
         <n v="12000"/>
@@ -5879,7 +5878,7 @@
         <m/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Laba" numFmtId="176">
+    <cacheField name="Laba" numFmtId="177">
       <sharedItems containsBlank="1" containsNumber="1" containsMixedTypes="1" count="103">
         <n v="-54150"/>
         <n v="-10450"/>
@@ -17123,276 +17122,276 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="74" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="76" t="s">
+      <c r="E3" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="78" t="s">
+      <c r="G3" s="77" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="79">
+      <c r="B4" s="78">
         <v>42862</v>
       </c>
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="80" t="s">
+      <c r="D4" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="80" t="s">
+      <c r="E4" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="80" t="s">
+      <c r="F4" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="78">
+      <c r="G4" s="77">
         <v>50000</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="82">
+      <c r="B5" s="81">
         <v>42883</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="83" t="s">
+      <c r="E5" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="83" t="s">
+      <c r="F5" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="84">
+      <c r="G5" s="83">
         <v>200000</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="82">
+      <c r="B6" s="81">
         <v>42920</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="83" t="s">
+      <c r="D6" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="83" t="s">
+      <c r="E6" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="83" t="s">
+      <c r="F6" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="84">
+      <c r="G6" s="83">
         <v>100000</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="82">
+      <c r="B7" s="81">
         <v>42946</v>
       </c>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="83" t="s">
+      <c r="D7" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="83" t="s">
+      <c r="E7" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="83" t="s">
+      <c r="F7" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="84">
+      <c r="G7" s="83">
         <v>100000</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="82">
+      <c r="B8" s="81">
         <v>42946</v>
       </c>
-      <c r="C8" s="83" t="s">
+      <c r="C8" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="83" t="s">
+      <c r="D8" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="83" t="s">
+      <c r="E8" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="83" t="s">
+      <c r="F8" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="84">
+      <c r="G8" s="83">
         <v>100000</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="81" t="s">
+      <c r="A9" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="82">
+      <c r="B9" s="81">
         <v>42962</v>
       </c>
-      <c r="C9" s="83" t="s">
+      <c r="C9" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="83" t="s">
+      <c r="D9" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="83" t="s">
+      <c r="E9" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="83" t="s">
+      <c r="F9" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="84">
+      <c r="G9" s="83">
         <v>100000</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="82">
+      <c r="B10" s="81">
         <v>42869</v>
       </c>
-      <c r="C10" s="83" t="s">
+      <c r="C10" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="83" t="s">
+      <c r="E10" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="83" t="s">
+      <c r="F10" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="84">
+      <c r="G10" s="83">
         <v>50500</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="82">
+      <c r="B11" s="81">
         <v>42882</v>
       </c>
-      <c r="C11" s="83" t="s">
+      <c r="C11" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="83" t="s">
+      <c r="D11" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="83" t="s">
+      <c r="E11" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="83" t="s">
+      <c r="F11" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="84">
+      <c r="G11" s="83">
         <v>50000</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="82">
+      <c r="B12" s="81">
         <v>42883</v>
       </c>
-      <c r="C12" s="83" t="s">
+      <c r="C12" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="83" t="s">
+      <c r="D12" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="83" t="s">
+      <c r="E12" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="83" t="s">
+      <c r="F12" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="84">
+      <c r="G12" s="83">
         <v>50500</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="82">
+      <c r="B13" s="81">
         <v>42938</v>
       </c>
-      <c r="C13" s="83" t="s">
+      <c r="C13" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="83" t="s">
+      <c r="D13" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="83" t="s">
+      <c r="E13" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="83" t="s">
+      <c r="F13" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="84">
+      <c r="G13" s="83">
         <v>50000</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="85" t="s">
+      <c r="A14" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="86"/>
-      <c r="C14" s="87"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="88">
+      <c r="B14" s="85"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="87">
         <v>851000</v>
       </c>
     </row>
@@ -17771,11 +17770,11 @@
   <dimension ref="A1:N643"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B627" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B219" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H640" sqref="H640"/>
+      <selection pane="bottomRight" activeCell="D227" sqref="D227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -22103,7 +22102,7 @@
       </c>
     </row>
     <row r="130" ht="30" spans="1:11">
-      <c r="A130" s="89" t="s">
+      <c r="A130" s="88" t="s">
         <v>259</v>
       </c>
       <c r="B130" s="48">
@@ -22140,7 +22139,7 @@
       </c>
     </row>
     <row r="131" ht="30" spans="1:11">
-      <c r="A131" s="89" t="s">
+      <c r="A131" s="88" t="s">
         <v>261</v>
       </c>
       <c r="B131" s="48">
@@ -22175,7 +22174,7 @@
       </c>
     </row>
     <row r="132" ht="30" spans="1:11">
-      <c r="A132" s="89" t="s">
+      <c r="A132" s="88" t="s">
         <v>264</v>
       </c>
       <c r="B132" s="48">
@@ -22212,7 +22211,7 @@
       </c>
     </row>
     <row r="133" ht="30" spans="1:11">
-      <c r="A133" s="89" t="s">
+      <c r="A133" s="88" t="s">
         <v>266</v>
       </c>
       <c r="B133" s="48">
@@ -22286,7 +22285,7 @@
       </c>
     </row>
     <row r="135" spans="1:11">
-      <c r="A135" s="89" t="s">
+      <c r="A135" s="88" t="s">
         <v>272</v>
       </c>
       <c r="B135" s="48">
@@ -22323,7 +22322,7 @@
       </c>
     </row>
     <row r="136" ht="30" spans="1:11">
-      <c r="A136" s="89" t="s">
+      <c r="A136" s="88" t="s">
         <v>273</v>
       </c>
       <c r="B136" s="48">
@@ -22360,7 +22359,7 @@
       </c>
     </row>
     <row r="137" ht="30" spans="1:11">
-      <c r="A137" s="89" t="s">
+      <c r="A137" s="88" t="s">
         <v>276</v>
       </c>
       <c r="B137" s="48">
@@ -22397,7 +22396,7 @@
       </c>
     </row>
     <row r="138" spans="1:11">
-      <c r="A138" s="89" t="s">
+      <c r="A138" s="88" t="s">
         <v>278</v>
       </c>
       <c r="B138" s="48">
@@ -22431,7 +22430,7 @@
       </c>
     </row>
     <row r="139" spans="1:11">
-      <c r="A139" s="89" t="s">
+      <c r="A139" s="88" t="s">
         <v>279</v>
       </c>
       <c r="B139" s="48">
@@ -22690,7 +22689,7 @@
       </c>
     </row>
     <row r="146" spans="1:11">
-      <c r="A146" s="89" t="s">
+      <c r="A146" s="88" t="s">
         <v>289</v>
       </c>
       <c r="B146" s="48">
@@ -22724,7 +22723,7 @@
       </c>
     </row>
     <row r="147" spans="1:11">
-      <c r="A147" s="89" t="s">
+      <c r="A147" s="88" t="s">
         <v>292</v>
       </c>
       <c r="B147" s="48">
@@ -22758,7 +22757,7 @@
       </c>
     </row>
     <row r="148" spans="1:11">
-      <c r="A148" s="89" t="s">
+      <c r="A148" s="88" t="s">
         <v>294</v>
       </c>
       <c r="B148" s="48">
@@ -22792,7 +22791,7 @@
       </c>
     </row>
     <row r="149" spans="1:11">
-      <c r="A149" s="89" t="s">
+      <c r="A149" s="88" t="s">
         <v>296</v>
       </c>
       <c r="B149" s="48">
@@ -22826,7 +22825,7 @@
       </c>
     </row>
     <row r="150" spans="1:11">
-      <c r="A150" s="89" t="s">
+      <c r="A150" s="88" t="s">
         <v>9</v>
       </c>
       <c r="B150" s="48">
@@ -22860,7 +22859,7 @@
       </c>
     </row>
     <row r="151" spans="1:11">
-      <c r="A151" s="89" t="s">
+      <c r="A151" s="88" t="s">
         <v>298</v>
       </c>
       <c r="B151" s="48">
@@ -22931,7 +22930,7 @@
       </c>
     </row>
     <row r="153" spans="1:11">
-      <c r="A153" s="89" t="s">
+      <c r="A153" s="88" t="s">
         <v>304</v>
       </c>
       <c r="B153" s="48">
@@ -22965,7 +22964,7 @@
       </c>
     </row>
     <row r="154" spans="1:11">
-      <c r="A154" s="89" t="s">
+      <c r="A154" s="88" t="s">
         <v>305</v>
       </c>
       <c r="B154" s="48">
@@ -23036,7 +23035,7 @@
       </c>
     </row>
     <row r="156" spans="1:11">
-      <c r="A156" s="89" t="s">
+      <c r="A156" s="88" t="s">
         <v>310</v>
       </c>
       <c r="B156" s="48">
@@ -23107,7 +23106,7 @@
       </c>
     </row>
     <row r="158" spans="1:11">
-      <c r="A158" s="89" t="s">
+      <c r="A158" s="88" t="s">
         <v>313</v>
       </c>
       <c r="B158" s="48">
@@ -23178,7 +23177,7 @@
       </c>
     </row>
     <row r="160" spans="1:11">
-      <c r="A160" s="89" t="s">
+      <c r="A160" s="88" t="s">
         <v>315</v>
       </c>
       <c r="B160" s="48">
@@ -23249,7 +23248,7 @@
       </c>
     </row>
     <row r="162" spans="1:11">
-      <c r="A162" s="89" t="s">
+      <c r="A162" s="88" t="s">
         <v>319</v>
       </c>
       <c r="B162" s="48">
@@ -23283,7 +23282,7 @@
       </c>
     </row>
     <row r="163" spans="1:11">
-      <c r="A163" s="89" t="s">
+      <c r="A163" s="88" t="s">
         <v>320</v>
       </c>
       <c r="B163" s="48">
@@ -23317,7 +23316,7 @@
       </c>
     </row>
     <row r="164" spans="1:11">
-      <c r="A164" s="89" t="s">
+      <c r="A164" s="88" t="s">
         <v>321</v>
       </c>
       <c r="B164" s="48">
@@ -23348,7 +23347,7 @@
       </c>
     </row>
     <row r="165" spans="1:11">
-      <c r="A165" s="89" t="s">
+      <c r="A165" s="88" t="s">
         <v>324</v>
       </c>
       <c r="B165" s="48">
@@ -23382,7 +23381,7 @@
       </c>
     </row>
     <row r="166" spans="1:11">
-      <c r="A166" s="89" t="s">
+      <c r="A166" s="88" t="s">
         <v>325</v>
       </c>
       <c r="B166" s="48">
@@ -23416,7 +23415,7 @@
       </c>
     </row>
     <row r="167" spans="1:11">
-      <c r="A167" s="89" t="s">
+      <c r="A167" s="88" t="s">
         <v>328</v>
       </c>
       <c r="B167" s="48">
@@ -23580,7 +23579,7 @@
       </c>
     </row>
     <row r="172" spans="1:11">
-      <c r="A172" s="89" t="s">
+      <c r="A172" s="88" t="s">
         <v>336</v>
       </c>
       <c r="B172" s="48">
@@ -24632,7 +24631,7 @@
       <c r="C201" t="s">
         <v>120</v>
       </c>
-      <c r="D201" s="90" t="s">
+      <c r="D201" s="89" t="s">
         <v>378</v>
       </c>
       <c r="F201" s="18">
@@ -26044,7 +26043,7 @@
       <c r="C242" t="s">
         <v>454</v>
       </c>
-      <c r="D242" s="90" t="s">
+      <c r="D242" s="89" t="s">
         <v>378</v>
       </c>
       <c r="F242" s="18">
@@ -27704,7 +27703,7 @@
       <c r="C291" t="s">
         <v>35</v>
       </c>
-      <c r="D291" s="90" t="s">
+      <c r="D291" s="89" t="s">
         <v>155</v>
       </c>
       <c r="E291" t="s">
@@ -28013,7 +28012,7 @@
       <c r="C300" t="s">
         <v>454</v>
       </c>
-      <c r="D300" s="90" t="s">
+      <c r="D300" s="89" t="s">
         <v>378</v>
       </c>
       <c r="F300" s="18">
@@ -37261,7 +37260,7 @@
       <c r="C562" t="s">
         <v>866</v>
       </c>
-      <c r="D562" s="90" t="s">
+      <c r="D562" s="89" t="s">
         <v>867</v>
       </c>
       <c r="E562" s="41" t="s">
@@ -39817,7 +39816,7 @@
       </c>
     </row>
     <row r="634" ht="30" spans="1:11">
-      <c r="A634" s="73" t="s">
+      <c r="A634" s="62" t="s">
         <v>951</v>
       </c>
       <c r="B634" s="48">
@@ -39854,7 +39853,7 @@
       </c>
     </row>
     <row r="635" ht="30" spans="1:11">
-      <c r="A635" s="73" t="s">
+      <c r="A635" s="62" t="s">
         <v>952</v>
       </c>
       <c r="B635" s="48">
@@ -39891,7 +39890,7 @@
       </c>
     </row>
     <row r="636" spans="1:11">
-      <c r="A636" s="73" t="s">
+      <c r="A636" s="62" t="s">
         <v>953</v>
       </c>
       <c r="B636" s="48">
@@ -39925,7 +39924,7 @@
       </c>
     </row>
     <row r="637" spans="1:11">
-      <c r="A637" s="73" t="s">
+      <c r="A637" s="62" t="s">
         <v>954</v>
       </c>
       <c r="B637" s="48">
@@ -39962,7 +39961,7 @@
       </c>
     </row>
     <row r="638" spans="1:11">
-      <c r="A638" s="73" t="s">
+      <c r="A638" s="62" t="s">
         <v>955</v>
       </c>
       <c r="B638" s="48">
@@ -39978,7 +39977,7 @@
       </c>
     </row>
     <row r="639" spans="1:11">
-      <c r="A639" s="73" t="s">
+      <c r="A639" s="62" t="s">
         <v>956</v>
       </c>
       <c r="B639" s="48">
@@ -39994,7 +39993,7 @@
       </c>
     </row>
     <row r="640" spans="1:11">
-      <c r="A640" s="73" t="s">
+      <c r="A640" s="62" t="s">
         <v>957</v>
       </c>
       <c r="B640" s="48">
@@ -40040,7 +40039,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:I633"/>
+  <autoFilter ref="B1:I640"/>
   <hyperlinks>
     <hyperlink ref="A173" r:id="rId1" display="BL171111JKC7ELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/795416"/>
     <hyperlink ref="A174" r:id="rId2" display="BL171111JMU2ELC" tooltip="https://www.bukalapak.com/payment/electricity/transactions/798491"/>
@@ -41524,7 +41523,7 @@
       </c>
     </row>
     <row r="7" ht="30" hidden="1" spans="1:9">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="88" t="s">
         <v>261</v>
       </c>
       <c r="B7" s="15">

</xml_diff>